<commit_message>
Added hours for sprint 3
</commit_message>
<xml_diff>
--- a/Management/Effort and Velocity.xlsx
+++ b/Management/Effort and Velocity.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="295"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="295" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
     <sheet name="Sp1" sheetId="3" r:id="rId2"/>
     <sheet name="Sp2" sheetId="4" r:id="rId3"/>
+    <sheet name="Sp3" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="45">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -143,6 +147,15 @@
   <si>
     <t>Week 4</t>
   </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
 </sst>
 </file>
 
@@ -255,7 +268,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -765,11 +778,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -927,9 +970,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -943,9 +983,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1036,7 +1073,43 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1057,30 +1130,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1093,25 +1142,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1150,15 +1187,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1526,13 +1613,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="75844992"/>
-        <c:axId val="85931136"/>
+        <c:axId val="273211128"/>
+        <c:axId val="273206424"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="75844992"/>
+        <c:axId val="273211128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1542,14 +1628,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85931136"/>
+        <c:crossAx val="273206424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="85931136"/>
+        <c:axId val="273206424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1560,7 +1646,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75844992"/>
+        <c:crossAx val="273211128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1831,13 +1917,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="85999616"/>
-        <c:axId val="86001152"/>
+        <c:axId val="335893024"/>
+        <c:axId val="335892632"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="85999616"/>
+        <c:axId val="335893024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1847,14 +1932,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86001152"/>
+        <c:crossAx val="335892632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="86001152"/>
+        <c:axId val="335892632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1865,7 +1950,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85999616"/>
+        <c:crossAx val="335893024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2136,13 +2221,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="86010112"/>
-        <c:axId val="86020096"/>
+        <c:axId val="335893808"/>
+        <c:axId val="335894200"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="86010112"/>
+        <c:axId val="335893808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2152,14 +2236,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86020096"/>
+        <c:crossAx val="335894200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="86020096"/>
+        <c:axId val="335894200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2170,7 +2254,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86010112"/>
+        <c:crossAx val="335893808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2444,13 +2528,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="86053632"/>
-        <c:axId val="86055168"/>
+        <c:axId val="336474840"/>
+        <c:axId val="336473664"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="86053632"/>
+        <c:axId val="336474840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2460,14 +2543,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86055168"/>
+        <c:crossAx val="336473664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="86055168"/>
+        <c:axId val="336473664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2478,7 +2561,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86053632"/>
+        <c:crossAx val="336474840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2713,13 +2796,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="86101376"/>
-        <c:axId val="86107264"/>
+        <c:axId val="336475624"/>
+        <c:axId val="336477192"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="86101376"/>
+        <c:axId val="336475624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2729,14 +2811,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86107264"/>
+        <c:crossAx val="336477192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="86107264"/>
+        <c:axId val="336477192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2747,7 +2829,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86101376"/>
+        <c:crossAx val="336475624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2982,13 +3064,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="86345600"/>
-        <c:axId val="86347136"/>
+        <c:axId val="336477584"/>
+        <c:axId val="336473272"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="86345600"/>
+        <c:axId val="336477584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2998,14 +3079,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86347136"/>
+        <c:crossAx val="336473272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="86347136"/>
+        <c:axId val="336473272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3016,7 +3097,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86345600"/>
+        <c:crossAx val="336477584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3251,13 +3332,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="88621440"/>
-        <c:axId val="88622976"/>
+        <c:axId val="336476016"/>
+        <c:axId val="336478368"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="88621440"/>
+        <c:axId val="336476016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3267,14 +3347,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88622976"/>
+        <c:crossAx val="336478368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="88622976"/>
+        <c:axId val="336478368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3285,7 +3365,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88621440"/>
+        <c:crossAx val="336476016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3520,13 +3600,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="88660608"/>
-        <c:axId val="88662400"/>
+        <c:axId val="336474056"/>
+        <c:axId val="336477976"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="88660608"/>
+        <c:axId val="336474056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3536,14 +3615,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88662400"/>
+        <c:crossAx val="336477976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="88662400"/>
+        <c:axId val="336477976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3554,7 +3633,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88660608"/>
+        <c:crossAx val="336474056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3938,13 +4017,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69957888"/>
-        <c:axId val="69959680"/>
+        <c:axId val="273209560"/>
+        <c:axId val="273204856"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="69957888"/>
+        <c:axId val="273209560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3954,14 +4032,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69959680"/>
+        <c:crossAx val="273204856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="69959680"/>
+        <c:axId val="273204856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3972,7 +4050,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69957888"/>
+        <c:crossAx val="273209560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4356,13 +4434,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="85721856"/>
-        <c:axId val="85723392"/>
+        <c:axId val="273206032"/>
+        <c:axId val="273204072"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="85721856"/>
+        <c:axId val="273206032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4372,14 +4449,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85723392"/>
+        <c:crossAx val="273204072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="85723392"/>
+        <c:axId val="273204072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4390,7 +4467,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85721856"/>
+        <c:crossAx val="273206032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4774,13 +4851,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="85736448"/>
-        <c:axId val="85742336"/>
+        <c:axId val="273208384"/>
+        <c:axId val="139700592"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="85736448"/>
+        <c:axId val="273208384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4790,14 +4866,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85742336"/>
+        <c:crossAx val="139700592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="85742336"/>
+        <c:axId val="139700592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4808,7 +4884,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85736448"/>
+        <c:crossAx val="273208384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4988,13 +5064,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="85753856"/>
-        <c:axId val="85755392"/>
+        <c:axId val="335891848"/>
+        <c:axId val="335886752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85753856"/>
+        <c:axId val="335891848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5004,7 +5079,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85755392"/>
+        <c:crossAx val="335886752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5012,7 +5087,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85755392"/>
+        <c:axId val="335886752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5023,7 +5098,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85753856"/>
+        <c:crossAx val="335891848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5203,13 +5278,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="85772928"/>
-        <c:axId val="85778816"/>
+        <c:axId val="335888712"/>
+        <c:axId val="335890672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85772928"/>
+        <c:axId val="335888712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5219,7 +5293,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85778816"/>
+        <c:crossAx val="335890672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5227,7 +5301,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85778816"/>
+        <c:axId val="335890672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5238,7 +5312,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85772928"/>
+        <c:crossAx val="335888712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5418,13 +5492,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="85857408"/>
-        <c:axId val="85858944"/>
+        <c:axId val="335889496"/>
+        <c:axId val="335889888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85857408"/>
+        <c:axId val="335889496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5434,7 +5507,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85858944"/>
+        <c:crossAx val="335889888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5442,7 +5515,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85858944"/>
+        <c:axId val="335889888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5453,7 +5526,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85857408"/>
+        <c:crossAx val="335889496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5633,13 +5706,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="85876096"/>
-        <c:axId val="85894272"/>
+        <c:axId val="335887536"/>
+        <c:axId val="335887928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85876096"/>
+        <c:axId val="335887536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5649,7 +5721,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85894272"/>
+        <c:crossAx val="335887928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5657,7 +5729,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85894272"/>
+        <c:axId val="335887928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5668,7 +5740,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85876096"/>
+        <c:crossAx val="335887536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5939,13 +6011,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="85960576"/>
-        <c:axId val="85962112"/>
+        <c:axId val="335891064"/>
+        <c:axId val="335891456"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="85960576"/>
+        <c:axId val="335891064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5955,14 +6026,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85962112"/>
+        <c:crossAx val="335891456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="85962112"/>
+        <c:axId val="335891456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5973,7 +6044,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85960576"/>
+        <c:crossAx val="335891064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6561,7 +6632,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6596,7 +6667,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6805,10 +6876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:X36"/>
+  <dimension ref="B2:AH36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6816,65 +6887,91 @@
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="D2" s="106" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="108"/>
-      <c r="P2" s="106" t="s">
+    <row r="2" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="D2" s="102" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="107"/>
-      <c r="S2" s="107"/>
-      <c r="T2" s="107"/>
-      <c r="U2" s="107"/>
-      <c r="V2" s="107"/>
-      <c r="W2" s="107"/>
-      <c r="X2" s="108"/>
+      <c r="Q2" s="103"/>
+      <c r="R2" s="103"/>
+      <c r="S2" s="103"/>
+      <c r="T2" s="103"/>
+      <c r="U2" s="103"/>
+      <c r="V2" s="103"/>
+      <c r="W2" s="103"/>
+      <c r="X2" s="104"/>
+      <c r="Y2" s="102" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z2" s="103"/>
+      <c r="AA2" s="103"/>
+      <c r="AB2" s="103"/>
+      <c r="AC2" s="103"/>
+      <c r="AD2" s="103"/>
+      <c r="AE2" s="103"/>
+      <c r="AF2" s="103"/>
+      <c r="AG2" s="103"/>
+      <c r="AH2" s="104"/>
     </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="D3" s="112" t="s">
+    <row r="3" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="D3" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="113"/>
-      <c r="F3" s="113"/>
-      <c r="G3" s="113"/>
-      <c r="H3" s="113"/>
-      <c r="I3" s="113"/>
-      <c r="J3" s="106" t="s">
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="108"/>
-      <c r="P3" s="106" t="s">
+      <c r="K3" s="103"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="103"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="107"/>
-      <c r="R3" s="107"/>
-      <c r="S3" s="107"/>
-      <c r="T3" s="107"/>
-      <c r="U3" s="106" t="s">
+      <c r="Q3" s="103"/>
+      <c r="R3" s="103"/>
+      <c r="S3" s="103"/>
+      <c r="T3" s="103"/>
+      <c r="U3" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="107"/>
-      <c r="W3" s="107"/>
-      <c r="X3" s="108"/>
+      <c r="V3" s="103"/>
+      <c r="W3" s="103"/>
+      <c r="X3" s="104"/>
+      <c r="Y3" s="102" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z3" s="103"/>
+      <c r="AA3" s="103"/>
+      <c r="AB3" s="103"/>
+      <c r="AC3" s="103"/>
+      <c r="AD3" s="102" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE3" s="103"/>
+      <c r="AF3" s="103"/>
+      <c r="AG3" s="103"/>
+      <c r="AH3" s="104"/>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D4" s="1">
         <v>41939</v>
       </c>
@@ -6938,8 +7035,38 @@
       <c r="X4" s="1">
         <v>41983</v>
       </c>
+      <c r="Y4" s="1">
+        <v>42023</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>42024</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>42025</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>42026</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>42027</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>42030</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>42031</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>42032</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>42033</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>42034</v>
+      </c>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D5" s="4">
         <v>1</v>
       </c>
@@ -7003,9 +7130,39 @@
       <c r="X5" s="4">
         <v>21</v>
       </c>
+      <c r="Y5" s="3">
+        <v>22</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>23</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>24</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>25</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>26</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>27</v>
+      </c>
+      <c r="AE5" s="3">
+        <v>28</v>
+      </c>
+      <c r="AF5" s="3">
+        <v>29</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>30</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>31</v>
+      </c>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="114" t="s">
+    <row r="6" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B6" s="110" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
@@ -7083,9 +7240,19 @@
         <f>'Sp2'!L26</f>
         <v>0</v>
       </c>
+      <c r="Y6" s="78"/>
+      <c r="Z6" s="79"/>
+      <c r="AA6" s="79"/>
+      <c r="AB6" s="79"/>
+      <c r="AC6" s="79"/>
+      <c r="AD6" s="79"/>
+      <c r="AE6" s="79"/>
+      <c r="AF6" s="79"/>
+      <c r="AG6" s="79"/>
+      <c r="AH6" s="80"/>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B7" s="115"/>
+    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B7" s="111"/>
       <c r="C7" s="29" t="s">
         <v>8</v>
       </c>
@@ -7161,9 +7328,19 @@
         <f>'Sp2'!L27</f>
         <v>0</v>
       </c>
+      <c r="Y7" s="65"/>
+      <c r="Z7" s="63"/>
+      <c r="AA7" s="63"/>
+      <c r="AB7" s="63"/>
+      <c r="AC7" s="63"/>
+      <c r="AD7" s="63"/>
+      <c r="AE7" s="63"/>
+      <c r="AF7" s="63"/>
+      <c r="AG7" s="63"/>
+      <c r="AH7" s="66"/>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B8" s="115"/>
+    <row r="8" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B8" s="111"/>
       <c r="C8" s="30" t="s">
         <v>9</v>
       </c>
@@ -7239,9 +7416,39 @@
         <f>'Sp2'!L28</f>
         <v>0</v>
       </c>
+      <c r="Y8" s="65">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="63">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="63">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="63">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="63">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="63">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="63">
+        <v>4.75</v>
+      </c>
+      <c r="AF8" s="63">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="63">
+        <v>2.75</v>
+      </c>
+      <c r="AH8" s="66">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B9" s="116"/>
+    <row r="9" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B9" s="112"/>
       <c r="C9" s="69" t="s">
         <v>4</v>
       </c>
@@ -7281,44 +7488,84 @@
       <c r="O9" s="74">
         <v>0</v>
       </c>
-      <c r="P9" s="81">
+      <c r="P9" s="72">
         <f>'Sp2'!D25</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="82">
+      <c r="Q9" s="73">
         <f>'Sp2'!E25</f>
         <v>4</v>
       </c>
-      <c r="R9" s="82">
+      <c r="R9" s="73">
         <f>'Sp2'!F25</f>
         <v>0</v>
       </c>
-      <c r="S9" s="82">
+      <c r="S9" s="73">
         <f>'Sp2'!G25</f>
         <v>0</v>
       </c>
-      <c r="T9" s="82">
+      <c r="T9" s="73">
         <f>'Sp2'!H25</f>
         <v>10</v>
       </c>
-      <c r="U9" s="82">
+      <c r="U9" s="73">
         <f>'Sp2'!I25</f>
         <v>18</v>
       </c>
-      <c r="V9" s="82">
+      <c r="V9" s="73">
         <f>'Sp2'!J25</f>
         <v>0</v>
       </c>
-      <c r="W9" s="82">
+      <c r="W9" s="73">
         <f>'Sp2'!K25</f>
         <v>0</v>
       </c>
-      <c r="X9" s="83">
+      <c r="X9" s="74">
         <f>'Sp2'!L25</f>
         <v>0</v>
       </c>
+      <c r="Y9" s="72">
+        <f>SUM(Y6:Y8)</f>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="72">
+        <f t="shared" ref="Z9:AH9" si="0">SUM(Z6:Z8)</f>
+        <v>0</v>
+      </c>
+      <c r="AA9" s="72">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AB9" s="72">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AC9" s="72">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD9" s="72">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE9" s="72">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
+      </c>
+      <c r="AF9" s="72">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AG9" s="72">
+        <f t="shared" si="0"/>
+        <v>2.75</v>
+      </c>
+      <c r="AH9" s="72">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="D10" s="67"/>
       <c r="E10" s="57"/>
@@ -7342,8 +7589,8 @@
       <c r="W10" s="57"/>
       <c r="X10" s="68"/>
     </row>
-    <row r="11" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="114" t="s">
+    <row r="11" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="110" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="28" t="s">
@@ -7428,13 +7675,23 @@
         <f>AVERAGE($D$6:W6)</f>
         <v>0.78749999999999998</v>
       </c>
-      <c r="X11" s="37">
+      <c r="X11" s="33">
         <f>AVERAGE($D$6:X6)</f>
         <v>0.75</v>
       </c>
+      <c r="Y11" s="58"/>
+      <c r="Z11" s="81"/>
+      <c r="AA11" s="81"/>
+      <c r="AB11" s="81"/>
+      <c r="AC11" s="81"/>
+      <c r="AD11" s="81"/>
+      <c r="AE11" s="81"/>
+      <c r="AF11" s="81"/>
+      <c r="AG11" s="81"/>
+      <c r="AH11" s="82"/>
     </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B12" s="115"/>
+    <row r="12" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B12" s="111"/>
       <c r="C12" s="29" t="s">
         <v>8</v>
       </c>
@@ -7517,13 +7774,23 @@
         <f>AVERAGE($D$7:W7)</f>
         <v>1.5</v>
       </c>
-      <c r="X12" s="39">
+      <c r="X12" s="38">
         <f>AVERAGE($D$7:X7)</f>
         <v>1.4285714285714286</v>
       </c>
+      <c r="Y12" s="67"/>
+      <c r="Z12" s="57"/>
+      <c r="AA12" s="57"/>
+      <c r="AB12" s="57"/>
+      <c r="AC12" s="57"/>
+      <c r="AD12" s="57"/>
+      <c r="AE12" s="57"/>
+      <c r="AF12" s="57"/>
+      <c r="AG12" s="57"/>
+      <c r="AH12" s="68"/>
     </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B13" s="115"/>
+    <row r="13" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B13" s="111"/>
       <c r="C13" s="30" t="s">
         <v>9</v>
       </c>
@@ -7606,101 +7873,181 @@
         <f>AVERAGE($D$8:W8)</f>
         <v>0.1</v>
       </c>
-      <c r="X13" s="39">
+      <c r="X13" s="38">
         <f>AVERAGE($D$8:X8)</f>
         <v>9.5238095238095233E-2</v>
       </c>
+      <c r="Y13" s="169">
+        <f>AVERAGE(D8:Y8)</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="Z13" s="38">
+        <f t="shared" ref="Z13:AH13" si="1">AVERAGE(E8:Z8)</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="AA13" s="38">
+        <f t="shared" si="1"/>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="AB13" s="38">
+        <f t="shared" si="1"/>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="AC13" s="38">
+        <f t="shared" si="1"/>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="AD13" s="38">
+        <f t="shared" si="1"/>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="AE13" s="38">
+        <f t="shared" si="1"/>
+        <v>0.35227272727272729</v>
+      </c>
+      <c r="AF13" s="38">
+        <f t="shared" si="1"/>
+        <v>0.28409090909090912</v>
+      </c>
+      <c r="AG13" s="38">
+        <f t="shared" si="1"/>
+        <v>0.38636363636363635</v>
+      </c>
+      <c r="AH13" s="39">
+        <f t="shared" si="1"/>
+        <v>0.40909090909090912</v>
+      </c>
     </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="116"/>
+    <row r="14" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B14" s="112"/>
       <c r="C14" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="86">
+      <c r="D14" s="83">
         <v>0.75</v>
       </c>
-      <c r="E14" s="89">
+      <c r="E14" s="86">
         <f>AVERAGE($D$9:E9)</f>
         <v>0.375</v>
       </c>
-      <c r="F14" s="89">
+      <c r="F14" s="86">
         <f>AVERAGE($D$9:F9)</f>
         <v>0.25</v>
       </c>
-      <c r="G14" s="89">
+      <c r="G14" s="86">
         <f>AVERAGE($D$9:G9)</f>
         <v>0.1875</v>
       </c>
-      <c r="H14" s="89">
+      <c r="H14" s="86">
         <f>AVERAGE($D$9:H9)</f>
         <v>0.15</v>
       </c>
-      <c r="I14" s="89">
+      <c r="I14" s="86">
         <f>AVERAGE($D$9:I9)</f>
         <v>0.45833333333333331</v>
       </c>
-      <c r="J14" s="89">
+      <c r="J14" s="86">
         <f>AVERAGE($D$9:J9)</f>
         <v>1.4642857142857142</v>
       </c>
-      <c r="K14" s="89">
+      <c r="K14" s="86">
         <f>AVERAGE($D$9:K9)</f>
         <v>1.96875</v>
       </c>
-      <c r="L14" s="89">
+      <c r="L14" s="86">
         <f>AVERAGE($D$9:L9)</f>
         <v>1.75</v>
       </c>
-      <c r="M14" s="89">
+      <c r="M14" s="86">
         <f>AVERAGE($D$9:M9)</f>
         <v>1.575</v>
       </c>
-      <c r="N14" s="89">
+      <c r="N14" s="86">
         <f>AVERAGE($D$9:N9)</f>
         <v>1.4318181818181819</v>
       </c>
-      <c r="O14" s="90">
+      <c r="O14" s="87">
         <f>AVERAGE($D$9:O9)</f>
         <v>1.3125</v>
       </c>
-      <c r="P14" s="89">
+      <c r="P14" s="86">
         <f>AVERAGE($D$9:P9)</f>
         <v>1.2115384615384615</v>
       </c>
-      <c r="Q14" s="89">
+      <c r="Q14" s="86">
         <f>AVERAGE($D$9:Q9)</f>
         <v>1.4107142857142858</v>
       </c>
-      <c r="R14" s="89">
+      <c r="R14" s="86">
         <f>AVERAGE($D$9:R9)</f>
         <v>1.3166666666666667</v>
       </c>
-      <c r="S14" s="89">
+      <c r="S14" s="86">
         <f>AVERAGE($D$9:S9)</f>
         <v>1.234375</v>
       </c>
-      <c r="T14" s="89">
+      <c r="T14" s="86">
         <f>AVERAGE($D$9:T9)</f>
         <v>1.75</v>
       </c>
-      <c r="U14" s="89">
+      <c r="U14" s="86">
         <f>AVERAGE($D$9:U9)</f>
         <v>2.6527777777777777</v>
       </c>
-      <c r="V14" s="89">
+      <c r="V14" s="86">
         <f>AVERAGE($D$9:V9)</f>
         <v>2.513157894736842</v>
       </c>
-      <c r="W14" s="89">
+      <c r="W14" s="86">
         <f>AVERAGE($D$9:W9)</f>
         <v>2.3875000000000002</v>
       </c>
-      <c r="X14" s="90">
+      <c r="X14" s="86">
         <f>AVERAGE($D$9:X9)</f>
         <v>2.2738095238095237</v>
       </c>
+      <c r="Y14" s="170">
+        <f>AVERAGE(D9:Y9)</f>
+        <v>2.1704545454545454</v>
+      </c>
+      <c r="Z14" s="86">
+        <f t="shared" ref="Z14:AH14" si="2">AVERAGE(E9:Z9)</f>
+        <v>2.1363636363636362</v>
+      </c>
+      <c r="AA14" s="86">
+        <f t="shared" si="2"/>
+        <v>2.1818181818181817</v>
+      </c>
+      <c r="AB14" s="86">
+        <f t="shared" si="2"/>
+        <v>2.1818181818181817</v>
+      </c>
+      <c r="AC14" s="86">
+        <f t="shared" si="2"/>
+        <v>2.1818181818181817</v>
+      </c>
+      <c r="AD14" s="86">
+        <f t="shared" si="2"/>
+        <v>2.1818181818181817</v>
+      </c>
+      <c r="AE14" s="86">
+        <f t="shared" si="2"/>
+        <v>2.3068181818181817</v>
+      </c>
+      <c r="AF14" s="86">
+        <f t="shared" si="2"/>
+        <v>1.9659090909090908</v>
+      </c>
+      <c r="AG14" s="86">
+        <f t="shared" si="2"/>
+        <v>1.8409090909090908</v>
+      </c>
+      <c r="AH14" s="87">
+        <f t="shared" si="2"/>
+        <v>1.8636363636363635</v>
+      </c>
     </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="D15" s="67"/>
       <c r="E15" s="57"/>
@@ -7724,680 +8071,854 @@
       <c r="W15" s="57"/>
       <c r="X15" s="68"/>
     </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B16" s="109" t="s">
+    <row r="16" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B16" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="87" t="s">
+      <c r="C16" s="84" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="58">
         <f>D6</f>
         <v>0.75</v>
       </c>
-      <c r="E16" s="84">
+      <c r="E16" s="81">
         <f>D16+E6</f>
         <v>0.75</v>
       </c>
-      <c r="F16" s="84">
-        <f t="shared" ref="F16:P16" si="0">E16+F6</f>
+      <c r="F16" s="81">
+        <f t="shared" ref="F16:P16" si="3">E16+F6</f>
         <v>0.75</v>
       </c>
-      <c r="G16" s="84">
-        <f t="shared" si="0"/>
+      <c r="G16" s="81">
+        <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="H16" s="84">
-        <f t="shared" si="0"/>
+      <c r="H16" s="81">
+        <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="I16" s="84">
-        <f t="shared" si="0"/>
+      <c r="I16" s="81">
+        <f t="shared" si="3"/>
         <v>2.75</v>
       </c>
-      <c r="J16" s="84">
-        <f t="shared" si="0"/>
+      <c r="J16" s="81">
+        <f t="shared" si="3"/>
         <v>6.75</v>
       </c>
-      <c r="K16" s="84">
-        <f t="shared" si="0"/>
+      <c r="K16" s="81">
+        <f t="shared" si="3"/>
         <v>6.75</v>
       </c>
-      <c r="L16" s="84">
-        <f t="shared" si="0"/>
+      <c r="L16" s="81">
+        <f t="shared" si="3"/>
         <v>6.75</v>
       </c>
-      <c r="M16" s="84">
-        <f t="shared" si="0"/>
+      <c r="M16" s="81">
+        <f t="shared" si="3"/>
         <v>6.75</v>
       </c>
-      <c r="N16" s="84">
-        <f t="shared" si="0"/>
+      <c r="N16" s="81">
+        <f t="shared" si="3"/>
         <v>6.75</v>
       </c>
-      <c r="O16" s="85">
-        <f t="shared" si="0"/>
+      <c r="O16" s="81">
+        <f t="shared" si="3"/>
         <v>6.75</v>
       </c>
-      <c r="P16" s="85">
-        <f t="shared" si="0"/>
+      <c r="P16" s="58">
+        <f t="shared" si="3"/>
         <v>6.75</v>
       </c>
-      <c r="Q16" s="85">
-        <f t="shared" ref="Q16:Q19" si="1">P16+Q6</f>
+      <c r="Q16" s="81">
+        <f t="shared" ref="Q16:Q19" si="4">P16+Q6</f>
         <v>6.75</v>
       </c>
-      <c r="R16" s="85">
-        <f t="shared" ref="R16:R19" si="2">Q16+R6</f>
+      <c r="R16" s="81">
+        <f t="shared" ref="R16:R19" si="5">Q16+R6</f>
         <v>6.75</v>
       </c>
-      <c r="S16" s="85">
-        <f t="shared" ref="S16:S19" si="3">R16+S6</f>
+      <c r="S16" s="81">
+        <f t="shared" ref="S16:S19" si="6">R16+S6</f>
         <v>6.75</v>
       </c>
-      <c r="T16" s="85">
-        <f t="shared" ref="T16:T19" si="4">S16+T6</f>
+      <c r="T16" s="81">
+        <f t="shared" ref="T16:T19" si="7">S16+T6</f>
         <v>12.75</v>
       </c>
-      <c r="U16" s="85">
-        <f t="shared" ref="U16:U19" si="5">T16+U6</f>
+      <c r="U16" s="81">
+        <f t="shared" ref="U16:U19" si="8">T16+U6</f>
         <v>15.75</v>
       </c>
-      <c r="V16" s="85">
-        <f t="shared" ref="V16:V19" si="6">U16+V6</f>
+      <c r="V16" s="81">
+        <f t="shared" ref="V16:V19" si="9">U16+V6</f>
         <v>15.75</v>
       </c>
-      <c r="W16" s="85">
-        <f t="shared" ref="W16:W19" si="7">V16+W6</f>
+      <c r="W16" s="81">
+        <f t="shared" ref="W16:W19" si="10">V16+W6</f>
         <v>15.75</v>
       </c>
-      <c r="X16" s="85">
-        <f t="shared" ref="X16:X19" si="8">W16+X6</f>
+      <c r="X16" s="81">
+        <f t="shared" ref="X16:X19" si="11">W16+X6</f>
         <v>15.75</v>
       </c>
+      <c r="Y16" s="58"/>
+      <c r="Z16" s="81"/>
+      <c r="AA16" s="81"/>
+      <c r="AB16" s="81"/>
+      <c r="AC16" s="81"/>
+      <c r="AD16" s="81"/>
+      <c r="AE16" s="81"/>
+      <c r="AF16" s="81"/>
+      <c r="AG16" s="81"/>
+      <c r="AH16" s="82"/>
     </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B17" s="110"/>
+    <row r="17" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B17" s="106"/>
       <c r="C17" s="70" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="67">
-        <f t="shared" ref="D17:D19" si="9">D7</f>
+        <f t="shared" ref="D17:D19" si="12">D7</f>
         <v>0</v>
       </c>
       <c r="E17" s="57">
-        <f t="shared" ref="E17:P19" si="10">D17+E7</f>
+        <f t="shared" ref="E17:P19" si="13">D17+E7</f>
         <v>0</v>
       </c>
       <c r="F17" s="57">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="57">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="57">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="57">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="57">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="K17" s="57">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="L17" s="57">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="M17" s="57">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="N17" s="57">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="O17" s="57">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="P17" s="67">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="Q17" s="57">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="R17" s="57">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="S17" s="57">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="T17" s="57">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="U17" s="57">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="V17" s="57">
+        <f t="shared" si="9"/>
+        <v>30</v>
+      </c>
+      <c r="W17" s="57">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="57">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="57">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="57">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="57">
+        <v>30</v>
+      </c>
+      <c r="X17" s="57">
+        <f t="shared" si="11"/>
+        <v>30</v>
+      </c>
+      <c r="Y17" s="67"/>
+      <c r="Z17" s="57"/>
+      <c r="AA17" s="57"/>
+      <c r="AB17" s="57"/>
+      <c r="AC17" s="57"/>
+      <c r="AD17" s="57"/>
+      <c r="AE17" s="57"/>
+      <c r="AF17" s="57"/>
+      <c r="AG17" s="57"/>
+      <c r="AH17" s="68"/>
+    </row>
+    <row r="18" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B18" s="106"/>
+      <c r="C18" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="67">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="57">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="57">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="57">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="57">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="57">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="57">
+        <f t="shared" si="13"/>
+        <v>1.5</v>
+      </c>
+      <c r="K18" s="57">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="L18" s="57">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="M18" s="57">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="N18" s="57">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="O18" s="57">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="P18" s="67">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="Q18" s="57">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="R18" s="57">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="S18" s="57">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="T18" s="57">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="U18" s="57">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="V18" s="57">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="W18" s="57">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="K17" s="57">
-        <f t="shared" si="10"/>
-        <v>7</v>
-      </c>
-      <c r="L17" s="57">
-        <f t="shared" si="10"/>
-        <v>7</v>
-      </c>
-      <c r="M17" s="57">
-        <f t="shared" si="10"/>
-        <v>7</v>
-      </c>
-      <c r="N17" s="57">
-        <f t="shared" si="10"/>
-        <v>7</v>
-      </c>
-      <c r="O17" s="68">
-        <f t="shared" si="10"/>
-        <v>7</v>
-      </c>
-      <c r="P17" s="68">
-        <f t="shared" si="10"/>
-        <v>7</v>
-      </c>
-      <c r="Q17" s="68">
-        <f t="shared" si="1"/>
+      <c r="X18" s="57">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="Y18" s="67">
+        <f>SUM(Y8,X18)</f>
+        <v>2</v>
+      </c>
+      <c r="Z18" s="57">
+        <f t="shared" ref="Z18:AH18" si="14">SUM(Z8,Y18)</f>
+        <v>2</v>
+      </c>
+      <c r="AA18" s="57">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="AB18" s="57">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="AC18" s="57">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="AD18" s="57">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="AE18" s="57">
+        <f t="shared" si="14"/>
+        <v>7.75</v>
+      </c>
+      <c r="AF18" s="57">
+        <f t="shared" si="14"/>
+        <v>7.75</v>
+      </c>
+      <c r="AG18" s="57">
+        <f t="shared" si="14"/>
+        <v>10.5</v>
+      </c>
+      <c r="AH18" s="68">
+        <f t="shared" si="14"/>
         <v>11</v>
       </c>
-      <c r="R17" s="68">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="S17" s="68">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-      <c r="T17" s="68">
+    </row>
+    <row r="19" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B19" s="107"/>
+      <c r="C19" s="85" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="72">
+        <f t="shared" si="12"/>
+        <v>0.75</v>
+      </c>
+      <c r="E19" s="73">
+        <f t="shared" si="13"/>
+        <v>0.75</v>
+      </c>
+      <c r="F19" s="73">
+        <f t="shared" si="13"/>
+        <v>0.75</v>
+      </c>
+      <c r="G19" s="73">
+        <f t="shared" si="13"/>
+        <v>0.75</v>
+      </c>
+      <c r="H19" s="73">
+        <f t="shared" si="13"/>
+        <v>0.75</v>
+      </c>
+      <c r="I19" s="73">
+        <f t="shared" si="13"/>
+        <v>2.75</v>
+      </c>
+      <c r="J19" s="73">
+        <f t="shared" si="13"/>
+        <v>10.25</v>
+      </c>
+      <c r="K19" s="73">
+        <f t="shared" si="13"/>
+        <v>15.75</v>
+      </c>
+      <c r="L19" s="73">
+        <f t="shared" si="13"/>
+        <v>15.75</v>
+      </c>
+      <c r="M19" s="73">
+        <f t="shared" si="13"/>
+        <v>15.75</v>
+      </c>
+      <c r="N19" s="73">
+        <f t="shared" si="13"/>
+        <v>15.75</v>
+      </c>
+      <c r="O19" s="73">
+        <f t="shared" si="13"/>
+        <v>15.75</v>
+      </c>
+      <c r="P19" s="72">
+        <f t="shared" si="13"/>
+        <v>15.75</v>
+      </c>
+      <c r="Q19" s="73">
         <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="U17" s="68">
+        <v>19.75</v>
+      </c>
+      <c r="R19" s="73">
         <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="V17" s="68">
+        <v>19.75</v>
+      </c>
+      <c r="S19" s="73">
         <f t="shared" si="6"/>
-        <v>30</v>
-      </c>
-      <c r="W17" s="68">
+        <v>19.75</v>
+      </c>
+      <c r="T19" s="73">
         <f t="shared" si="7"/>
-        <v>30</v>
-      </c>
-      <c r="X17" s="68">
-        <f t="shared" si="8"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B18" s="110"/>
-      <c r="C18" s="70" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="67">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="57">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="57">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="57">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="57">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="57">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="57">
-        <f t="shared" si="10"/>
-        <v>1.5</v>
-      </c>
-      <c r="K18" s="57">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="L18" s="57">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="M18" s="57">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="N18" s="57">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="O18" s="68">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="P18" s="68">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="Q18" s="68">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="R18" s="68">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="S18" s="68">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="T18" s="68">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="U18" s="68">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="V18" s="68">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="W18" s="68">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="X18" s="68">
-        <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B19" s="111"/>
-      <c r="C19" s="88" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="72">
-        <f t="shared" si="9"/>
-        <v>0.75</v>
-      </c>
-      <c r="E19" s="73">
-        <f t="shared" si="10"/>
-        <v>0.75</v>
-      </c>
-      <c r="F19" s="73">
-        <f t="shared" si="10"/>
-        <v>0.75</v>
-      </c>
-      <c r="G19" s="73">
-        <f t="shared" si="10"/>
-        <v>0.75</v>
-      </c>
-      <c r="H19" s="73">
-        <f t="shared" si="10"/>
-        <v>0.75</v>
-      </c>
-      <c r="I19" s="73">
-        <f t="shared" si="10"/>
-        <v>2.75</v>
-      </c>
-      <c r="J19" s="73">
-        <f t="shared" si="10"/>
-        <v>10.25</v>
-      </c>
-      <c r="K19" s="73">
-        <f t="shared" si="10"/>
-        <v>15.75</v>
-      </c>
-      <c r="L19" s="73">
-        <f t="shared" si="10"/>
-        <v>15.75</v>
-      </c>
-      <c r="M19" s="73">
-        <f t="shared" si="10"/>
-        <v>15.75</v>
-      </c>
-      <c r="N19" s="73">
-        <f t="shared" si="10"/>
-        <v>15.75</v>
-      </c>
-      <c r="O19" s="74">
-        <f t="shared" si="10"/>
-        <v>15.75</v>
-      </c>
-      <c r="P19" s="74">
-        <f t="shared" si="10"/>
-        <v>15.75</v>
-      </c>
-      <c r="Q19" s="74">
-        <f t="shared" si="1"/>
-        <v>19.75</v>
-      </c>
-      <c r="R19" s="74">
-        <f t="shared" si="2"/>
-        <v>19.75</v>
-      </c>
-      <c r="S19" s="74">
-        <f t="shared" si="3"/>
-        <v>19.75</v>
-      </c>
-      <c r="T19" s="74">
-        <f t="shared" si="4"/>
         <v>29.75</v>
       </c>
-      <c r="U19" s="74">
-        <f t="shared" si="5"/>
-        <v>47.75</v>
-      </c>
-      <c r="V19" s="74">
-        <f t="shared" si="6"/>
-        <v>47.75</v>
-      </c>
-      <c r="W19" s="74">
-        <f t="shared" si="7"/>
-        <v>47.75</v>
-      </c>
-      <c r="X19" s="74">
+      <c r="U19" s="73">
         <f t="shared" si="8"/>
         <v>47.75</v>
       </c>
+      <c r="V19" s="73">
+        <f t="shared" si="9"/>
+        <v>47.75</v>
+      </c>
+      <c r="W19" s="73">
+        <f t="shared" si="10"/>
+        <v>47.75</v>
+      </c>
+      <c r="X19" s="73">
+        <f t="shared" si="11"/>
+        <v>47.75</v>
+      </c>
+      <c r="Y19" s="72">
+        <f>SUM(Y16:Y18)</f>
+        <v>2</v>
+      </c>
+      <c r="Z19" s="73">
+        <f t="shared" ref="Z19:AH19" si="15">SUM(Z16:Z18)</f>
+        <v>2</v>
+      </c>
+      <c r="AA19" s="73">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="AB19" s="73">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="AC19" s="73">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="AD19" s="73">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="AE19" s="73">
+        <f t="shared" si="15"/>
+        <v>7.75</v>
+      </c>
+      <c r="AF19" s="73">
+        <f t="shared" si="15"/>
+        <v>7.75</v>
+      </c>
+      <c r="AG19" s="73">
+        <f t="shared" si="15"/>
+        <v>10.5</v>
+      </c>
+      <c r="AH19" s="74">
+        <f t="shared" si="15"/>
+        <v>11</v>
+      </c>
     </row>
-    <row r="21" spans="2:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="119" t="s">
+    <row r="21" spans="2:34" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="120"/>
-      <c r="D21" s="121">
+      <c r="C21" s="116"/>
+      <c r="D21" s="117">
         <v>1</v>
       </c>
-      <c r="E21" s="122"/>
-      <c r="F21" s="117">
+      <c r="E21" s="118"/>
+      <c r="F21" s="113">
         <v>2</v>
       </c>
-      <c r="G21" s="118"/>
+      <c r="G21" s="114"/>
+      <c r="H21" s="163">
+        <v>3</v>
+      </c>
+      <c r="I21" s="164"/>
     </row>
-    <row r="22" spans="2:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="123" t="s">
+    <row r="22" spans="2:34" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="124"/>
-      <c r="D22" s="101">
+      <c r="C22" s="120"/>
+      <c r="D22" s="97">
         <v>1</v>
       </c>
-      <c r="E22" s="102">
+      <c r="E22" s="98">
         <v>2</v>
       </c>
-      <c r="F22" s="100">
+      <c r="F22" s="96">
         <v>3</v>
       </c>
-      <c r="G22" s="91">
+      <c r="G22" s="162">
         <v>4</v>
       </c>
+      <c r="H22" s="165">
+        <v>5</v>
+      </c>
+      <c r="I22" s="166">
+        <v>6</v>
+      </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B23" s="109" t="s">
+    <row r="23" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B23" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="87" t="s">
+      <c r="C23" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="103">
+      <c r="D23" s="99">
         <f xml:space="preserve"> SUM(D6:I6)</f>
         <v>2.75</v>
       </c>
-      <c r="E23" s="95">
+      <c r="E23" s="91">
         <f xml:space="preserve"> SUM(J6:O6)</f>
         <v>4</v>
       </c>
-      <c r="F23" s="103">
+      <c r="F23" s="99">
         <f xml:space="preserve"> SUM(P6:T6)</f>
         <v>6</v>
       </c>
-      <c r="G23" s="95">
+      <c r="G23" s="91">
         <f xml:space="preserve"> SUM(U6:X6)</f>
         <v>3</v>
       </c>
+      <c r="H23" s="58"/>
+      <c r="I23" s="82"/>
     </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B24" s="110"/>
+    <row r="24" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B24" s="106"/>
       <c r="C24" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="104">
-        <f t="shared" ref="D24:D26" si="11" xml:space="preserve"> SUM(D7:I7)</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="97">
-        <f t="shared" ref="E24:E26" si="12" xml:space="preserve"> SUM(J7:O7)</f>
+      <c r="D24" s="100">
+        <f t="shared" ref="D24:D26" si="16" xml:space="preserve"> SUM(D7:I7)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="93">
+        <f t="shared" ref="E24:E26" si="17" xml:space="preserve"> SUM(J7:O7)</f>
         <v>7</v>
       </c>
-      <c r="F24" s="104">
-        <f t="shared" ref="F24:F26" si="13" xml:space="preserve"> SUM(P7:T7)</f>
+      <c r="F24" s="100">
+        <f t="shared" ref="F24:F26" si="18" xml:space="preserve"> SUM(P7:T7)</f>
         <v>8</v>
       </c>
-      <c r="G24" s="97">
-        <f t="shared" ref="G24:G26" si="14" xml:space="preserve"> SUM(U7:X7)</f>
+      <c r="G24" s="93">
+        <f t="shared" ref="G24:G26" si="19" xml:space="preserve"> SUM(U7:X7)</f>
         <v>15</v>
       </c>
+      <c r="H24" s="67"/>
+      <c r="I24" s="68"/>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B25" s="110"/>
+    <row r="25" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B25" s="106"/>
       <c r="C25" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="104">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="97">
-        <f t="shared" si="12"/>
+      <c r="D25" s="100">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="93">
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
-      <c r="F25" s="104">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="97">
-        <f t="shared" si="14"/>
-        <v>0</v>
+      <c r="F25" s="100">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="93">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="100">
+        <f>SUM(Y8:AC8)</f>
+        <v>1</v>
+      </c>
+      <c r="I25" s="93">
+        <f>SUM(AD8:AH8)</f>
+        <v>8</v>
       </c>
     </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B26" s="111"/>
-      <c r="C26" s="88" t="s">
+    <row r="26" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B26" s="107"/>
+      <c r="C26" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="105">
-        <f t="shared" si="11"/>
+      <c r="D26" s="101">
+        <f t="shared" si="16"/>
         <v>2.75</v>
       </c>
-      <c r="E26" s="99">
-        <f t="shared" si="12"/>
+      <c r="E26" s="95">
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
-      <c r="F26" s="105">
-        <f t="shared" si="13"/>
+      <c r="F26" s="101">
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
-      <c r="G26" s="99">
-        <f t="shared" si="14"/>
+      <c r="G26" s="95">
+        <f t="shared" si="19"/>
         <v>18</v>
       </c>
+      <c r="H26" s="167">
+        <f>SUM(H23:H25)</f>
+        <v>1</v>
+      </c>
+      <c r="I26" s="168">
+        <f>SUM(I23:I25)</f>
+        <v>8</v>
+      </c>
     </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B27" s="92"/>
-      <c r="C27" s="93"/>
+    <row r="27" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B27" s="88"/>
+      <c r="C27" s="89"/>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B28" s="125" t="s">
+    <row r="28" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B28" s="121" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="87" t="s">
+      <c r="C28" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="103">
+      <c r="D28" s="99">
         <f xml:space="preserve"> D23</f>
         <v>2.75</v>
       </c>
-      <c r="E28" s="95">
+      <c r="E28" s="91">
         <f xml:space="preserve"> AVERAGE($D$23:E23)</f>
         <v>3.375</v>
       </c>
-      <c r="F28" s="94">
+      <c r="F28" s="90">
         <f xml:space="preserve"> AVERAGE($D$23:F23)</f>
         <v>4.25</v>
       </c>
-      <c r="G28" s="95">
+      <c r="G28" s="90">
         <f xml:space="preserve"> AVERAGE($D$23:G23)</f>
         <v>3.9375</v>
       </c>
+      <c r="H28" s="58"/>
+      <c r="I28" s="82"/>
     </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B29" s="126"/>
+    <row r="29" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B29" s="122"/>
       <c r="C29" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="104">
-        <f t="shared" ref="D29:D31" si="15" xml:space="preserve"> D24</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="97">
+      <c r="D29" s="100">
+        <f t="shared" ref="D29:D31" si="20" xml:space="preserve"> D24</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="93">
         <f xml:space="preserve"> AVERAGE($D$24:E24)</f>
         <v>3.5</v>
       </c>
-      <c r="F29" s="96">
+      <c r="F29" s="92">
         <f xml:space="preserve"> AVERAGE($D$24:F24)</f>
         <v>5</v>
       </c>
-      <c r="G29" s="97">
+      <c r="G29" s="92">
         <f xml:space="preserve"> AVERAGE($D$24:G24)</f>
         <v>7.5</v>
       </c>
+      <c r="H29" s="67"/>
+      <c r="I29" s="68"/>
     </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B30" s="126"/>
+    <row r="30" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B30" s="122"/>
       <c r="C30" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="104">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="E30" s="97">
+      <c r="D30" s="100">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="93">
         <f xml:space="preserve"> AVERAGE($D$25:E25)</f>
         <v>1</v>
       </c>
-      <c r="F30" s="96">
+      <c r="F30" s="92">
         <f xml:space="preserve"> AVERAGE($D$25:F25)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="G30" s="97">
+      <c r="G30" s="92">
         <f xml:space="preserve"> AVERAGE($D$25:G25)</f>
         <v>0.5</v>
       </c>
+      <c r="H30" s="100">
+        <f>AVERAGE(D25:H25)</f>
+        <v>0.6</v>
+      </c>
+      <c r="I30" s="93">
+        <f>AVERAGE(E25:I25)</f>
+        <v>2.2000000000000002</v>
+      </c>
     </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B31" s="127"/>
-      <c r="C31" s="88" t="s">
+    <row r="31" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B31" s="123"/>
+      <c r="C31" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="105">
-        <f t="shared" si="15"/>
+      <c r="D31" s="101">
+        <f t="shared" si="20"/>
         <v>2.75</v>
       </c>
-      <c r="E31" s="99">
+      <c r="E31" s="95">
         <f xml:space="preserve"> AVERAGE($D$26:E26)</f>
         <v>7.875</v>
       </c>
-      <c r="F31" s="98">
+      <c r="F31" s="94">
         <f xml:space="preserve"> AVERAGE($D$26:F26)</f>
         <v>9.9166666666666661</v>
       </c>
-      <c r="G31" s="99">
+      <c r="G31" s="94">
         <f xml:space="preserve"> AVERAGE($D$26:G26)</f>
         <v>11.9375</v>
       </c>
+      <c r="H31" s="101">
+        <f>AVERAGE(D26:H26)</f>
+        <v>9.75</v>
+      </c>
+      <c r="I31" s="95">
+        <f>AVERAGE(E26:I26)</f>
+        <v>10.8</v>
+      </c>
     </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="109" t="s">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="105" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="87" t="s">
+      <c r="C33" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="103">
+      <c r="D33" s="99">
         <f xml:space="preserve"> D23</f>
         <v>2.75</v>
       </c>
-      <c r="E33" s="95">
+      <c r="E33" s="91">
         <f xml:space="preserve"> D33 + E23</f>
         <v>6.75</v>
       </c>
-      <c r="F33" s="94">
-        <f t="shared" ref="F33:G36" si="16" xml:space="preserve"> E33 + F23</f>
+      <c r="F33" s="90">
+        <f t="shared" ref="F33:G36" si="21" xml:space="preserve"> E33 + F23</f>
         <v>12.75</v>
       </c>
-      <c r="G33" s="95">
-        <f t="shared" si="16"/>
+      <c r="G33" s="90">
+        <f t="shared" si="21"/>
         <v>15.75</v>
       </c>
+      <c r="H33" s="58"/>
+      <c r="I33" s="82"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="110"/>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="106"/>
       <c r="C34" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="104">
-        <f t="shared" ref="D34:D36" si="17" xml:space="preserve"> D24</f>
-        <v>0</v>
-      </c>
-      <c r="E34" s="97">
-        <f t="shared" ref="E34:E36" si="18" xml:space="preserve"> D34 + E24</f>
+      <c r="D34" s="100">
+        <f t="shared" ref="D34:D36" si="22" xml:space="preserve"> D24</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="93">
+        <f t="shared" ref="E34:E36" si="23" xml:space="preserve"> D34 + E24</f>
         <v>7</v>
       </c>
-      <c r="F34" s="96">
-        <f t="shared" si="16"/>
+      <c r="F34" s="92">
+        <f t="shared" si="21"/>
         <v>15</v>
       </c>
-      <c r="G34" s="97">
-        <f t="shared" si="16"/>
+      <c r="G34" s="92">
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
+      <c r="H34" s="67"/>
+      <c r="I34" s="68"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="110"/>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="106"/>
       <c r="C35" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="104">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="E35" s="97">
-        <f t="shared" si="18"/>
+      <c r="D35" s="100">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="93">
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
-      <c r="F35" s="96">
-        <f t="shared" si="16"/>
+      <c r="F35" s="92">
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
-      <c r="G35" s="97">
-        <f t="shared" si="16"/>
+      <c r="G35" s="92">
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
+      <c r="H35" s="100">
+        <f>G35 + H25</f>
+        <v>3</v>
+      </c>
+      <c r="I35" s="93">
+        <f>H35 + I25</f>
+        <v>11</v>
+      </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="111"/>
-      <c r="C36" s="88" t="s">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="107"/>
+      <c r="C36" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="105">
-        <f t="shared" si="17"/>
+      <c r="D36" s="101">
+        <f t="shared" si="22"/>
         <v>2.75</v>
       </c>
-      <c r="E36" s="99">
-        <f t="shared" si="18"/>
+      <c r="E36" s="95">
+        <f t="shared" si="23"/>
         <v>15.75</v>
       </c>
-      <c r="F36" s="98">
-        <f t="shared" si="16"/>
+      <c r="F36" s="94">
+        <f t="shared" si="21"/>
         <v>29.75</v>
       </c>
-      <c r="G36" s="99">
-        <f t="shared" si="16"/>
+      <c r="G36" s="94">
+        <f t="shared" si="21"/>
         <v>47.75</v>
+      </c>
+      <c r="H36" s="101">
+        <f t="shared" ref="H36" si="24" xml:space="preserve"> G36 + H26</f>
+        <v>48.75</v>
+      </c>
+      <c r="I36" s="95">
+        <f t="shared" ref="I36" si="25" xml:space="preserve"> H36 + I26</f>
+        <v>56.75</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="20">
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="Y3:AC3"/>
+    <mergeCell ref="Y2:AH2"/>
+    <mergeCell ref="AD3:AH3"/>
     <mergeCell ref="P3:T3"/>
     <mergeCell ref="U3:X3"/>
     <mergeCell ref="P2:X2"/>
@@ -8428,7 +8949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -8439,22 +8960,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="113" t="s">
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
-      <c r="O1" s="147"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="109"/>
+      <c r="O1" s="124"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C2" s="6" t="s">
@@ -8562,10 +9083,10 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="137" t="s">
+      <c r="A5" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="148">
+      <c r="B5" s="125">
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -8625,8 +9146,8 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="138"/>
-      <c r="B6" s="149"/>
+      <c r="A6" s="132"/>
+      <c r="B6" s="126"/>
       <c r="C6" s="13" t="s">
         <v>7</v>
       </c>
@@ -8650,8 +9171,8 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="138"/>
-      <c r="B7" s="149"/>
+      <c r="A7" s="132"/>
+      <c r="B7" s="126"/>
       <c r="C7" s="13" t="s">
         <v>8</v>
       </c>
@@ -8675,8 +9196,8 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="138"/>
-      <c r="B8" s="149"/>
+      <c r="A8" s="132"/>
+      <c r="B8" s="126"/>
       <c r="C8" s="17" t="s">
         <v>9</v>
       </c>
@@ -8700,8 +9221,8 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="138"/>
-      <c r="B9" s="149"/>
+      <c r="A9" s="132"/>
+      <c r="B9" s="126"/>
       <c r="C9" s="21" t="s">
         <v>16</v>
       </c>
@@ -8759,8 +9280,8 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="138"/>
-      <c r="B10" s="149"/>
+      <c r="A10" s="132"/>
+      <c r="B10" s="126"/>
       <c r="C10" s="13" t="s">
         <v>7</v>
       </c>
@@ -8782,8 +9303,8 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="138"/>
-      <c r="B11" s="149"/>
+      <c r="A11" s="132"/>
+      <c r="B11" s="126"/>
       <c r="C11" s="13" t="s">
         <v>8</v>
       </c>
@@ -8805,8 +9326,8 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="138"/>
-      <c r="B12" s="149"/>
+      <c r="A12" s="132"/>
+      <c r="B12" s="126"/>
       <c r="C12" s="17" t="s">
         <v>9</v>
       </c>
@@ -8828,8 +9349,8 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="138"/>
-      <c r="B13" s="149"/>
+      <c r="A13" s="132"/>
+      <c r="B13" s="126"/>
       <c r="C13" s="21" t="s">
         <v>17</v>
       </c>
@@ -8887,8 +9408,8 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="138"/>
-      <c r="B14" s="149"/>
+      <c r="A14" s="132"/>
+      <c r="B14" s="126"/>
       <c r="C14" s="13" t="s">
         <v>7</v>
       </c>
@@ -8910,8 +9431,8 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="138"/>
-      <c r="B15" s="149"/>
+      <c r="A15" s="132"/>
+      <c r="B15" s="126"/>
       <c r="C15" s="13" t="s">
         <v>8</v>
       </c>
@@ -8933,8 +9454,8 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="138"/>
-      <c r="B16" s="150"/>
+      <c r="A16" s="132"/>
+      <c r="B16" s="127"/>
       <c r="C16" s="17" t="s">
         <v>9</v>
       </c>
@@ -8960,8 +9481,8 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="138"/>
-      <c r="B17" s="148">
+      <c r="A17" s="132"/>
+      <c r="B17" s="125">
         <v>3</v>
       </c>
       <c r="C17" s="21" t="s">
@@ -9021,8 +9542,8 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="138"/>
-      <c r="B18" s="149"/>
+      <c r="A18" s="132"/>
+      <c r="B18" s="126"/>
       <c r="C18" s="13" t="s">
         <v>7</v>
       </c>
@@ -9048,8 +9569,8 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="138"/>
-      <c r="B19" s="149"/>
+      <c r="A19" s="132"/>
+      <c r="B19" s="126"/>
       <c r="C19" s="13" t="s">
         <v>8</v>
       </c>
@@ -9071,8 +9592,8 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="138"/>
-      <c r="B20" s="150"/>
+      <c r="A20" s="132"/>
+      <c r="B20" s="127"/>
       <c r="C20" s="17" t="s">
         <v>9</v>
       </c>
@@ -9094,8 +9615,8 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="138"/>
-      <c r="B21" s="151"/>
+      <c r="A21" s="132"/>
+      <c r="B21" s="128"/>
       <c r="C21" s="21" t="s">
         <v>19</v>
       </c>
@@ -9153,8 +9674,8 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="138"/>
-      <c r="B22" s="152"/>
+      <c r="A22" s="132"/>
+      <c r="B22" s="129"/>
       <c r="C22" s="13" t="s">
         <v>7</v>
       </c>
@@ -9176,8 +9697,8 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="138"/>
-      <c r="B23" s="152"/>
+      <c r="A23" s="132"/>
+      <c r="B23" s="129"/>
       <c r="C23" s="13" t="s">
         <v>8</v>
       </c>
@@ -9201,8 +9722,8 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="139"/>
-      <c r="B24" s="153"/>
+      <c r="A24" s="133"/>
+      <c r="B24" s="130"/>
       <c r="C24" s="17" t="s">
         <v>9</v>
       </c>
@@ -9452,7 +9973,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="109" t="s">
+      <c r="A30" s="105" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="48" t="s">
@@ -9509,7 +10030,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="110"/>
+      <c r="A31" s="106"/>
       <c r="B31" s="50" t="s">
         <v>8</v>
       </c>
@@ -9564,7 +10085,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="110"/>
+      <c r="A32" s="106"/>
       <c r="B32" s="52" t="s">
         <v>9</v>
       </c>
@@ -9619,7 +10140,7 @@
       </c>
     </row>
     <row r="33" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="111"/>
+      <c r="A33" s="107"/>
       <c r="B33" s="145" t="s">
         <v>25</v>
       </c>
@@ -9688,13 +10209,13 @@
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="140" t="s">
+      <c r="A36" s="134" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="129" t="s">
+      <c r="B36" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="130"/>
+      <c r="C36" s="138"/>
       <c r="D36" s="26">
         <f xml:space="preserve"> SUM(D26:I26)</f>
         <v>2.75</v>
@@ -9709,11 +10230,11 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="141"/>
-      <c r="B37" s="131" t="s">
+      <c r="A37" s="135"/>
+      <c r="B37" s="139" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="132"/>
+      <c r="C37" s="140"/>
       <c r="D37" s="26">
         <f xml:space="preserve"> SUM(D27:I27)</f>
         <v>0</v>
@@ -9728,11 +10249,11 @@
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="141"/>
-      <c r="B38" s="133" t="s">
+      <c r="A38" s="135"/>
+      <c r="B38" s="141" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="134"/>
+      <c r="C38" s="142"/>
       <c r="D38" s="26">
         <f xml:space="preserve"> SUM(D28:I28)</f>
         <v>0</v>
@@ -9747,7 +10268,7 @@
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="142"/>
+      <c r="A39" s="136"/>
       <c r="B39" s="143" t="s">
         <v>25</v>
       </c>
@@ -9766,13 +10287,13 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="128" t="s">
+      <c r="A41" s="147" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="129" t="s">
+      <c r="B41" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="130"/>
+      <c r="C41" s="138"/>
       <c r="D41" s="31">
         <f xml:space="preserve"> D36</f>
         <v>2.75</v>
@@ -9783,11 +10304,11 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="128"/>
-      <c r="B42" s="131" t="s">
+      <c r="A42" s="147"/>
+      <c r="B42" s="139" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="132"/>
+      <c r="C42" s="140"/>
       <c r="D42" s="31">
         <f xml:space="preserve"> D37</f>
         <v>0</v>
@@ -9798,11 +10319,11 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="128"/>
-      <c r="B43" s="133" t="s">
+      <c r="A43" s="147"/>
+      <c r="B43" s="141" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="134"/>
+      <c r="C43" s="142"/>
       <c r="D43" s="31">
         <f xml:space="preserve"> D38</f>
         <v>0</v>
@@ -9813,11 +10334,11 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="128"/>
-      <c r="B44" s="135" t="s">
+      <c r="A44" s="147"/>
+      <c r="B44" s="148" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="136"/>
+      <c r="C44" s="149"/>
       <c r="D44" s="31">
         <f xml:space="preserve"> D39</f>
         <v>2.75</v>
@@ -9829,11 +10350,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="B5:B16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
     <mergeCell ref="A5:A24"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="B36:C36"/>
@@ -9842,11 +10363,11 @@
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="B5:B16"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9858,8 +10379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9870,19 +10391,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="106" t="s">
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="108"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="104"/>
       <c r="M1" s="54"/>
       <c r="N1" s="54"/>
       <c r="O1" s="55"/>
@@ -9984,10 +10505,10 @@
       <c r="P4" s="57"/>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="137" t="s">
+      <c r="A5" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="154">
+      <c r="B5" s="150">
         <v>1</v>
       </c>
       <c r="C5" s="59" t="s">
@@ -10035,8 +10556,8 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="138"/>
-      <c r="B6" s="155"/>
+      <c r="A6" s="132"/>
+      <c r="B6" s="151"/>
       <c r="C6" s="60" t="s">
         <v>7</v>
       </c>
@@ -10055,8 +10576,8 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="138"/>
-      <c r="B7" s="155"/>
+      <c r="A7" s="132"/>
+      <c r="B7" s="151"/>
       <c r="C7" s="60" t="s">
         <v>8</v>
       </c>
@@ -10081,8 +10602,8 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="138"/>
-      <c r="B8" s="156"/>
+      <c r="A8" s="132"/>
+      <c r="B8" s="152"/>
       <c r="C8" s="61" t="s">
         <v>9</v>
       </c>
@@ -10101,8 +10622,8 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="138"/>
-      <c r="B9" s="159" t="s">
+      <c r="A9" s="132"/>
+      <c r="B9" s="155" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="62" t="s">
@@ -10150,8 +10671,8 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="138"/>
-      <c r="B10" s="160"/>
+      <c r="A10" s="132"/>
+      <c r="B10" s="156"/>
       <c r="C10" s="60" t="s">
         <v>7</v>
       </c>
@@ -10174,8 +10695,8 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="138"/>
-      <c r="B11" s="160"/>
+      <c r="A11" s="132"/>
+      <c r="B11" s="156"/>
       <c r="C11" s="60" t="s">
         <v>8</v>
       </c>
@@ -10194,8 +10715,8 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="138"/>
-      <c r="B12" s="160"/>
+      <c r="A12" s="132"/>
+      <c r="B12" s="156"/>
       <c r="C12" s="61" t="s">
         <v>9</v>
       </c>
@@ -10214,8 +10735,8 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="138"/>
-      <c r="B13" s="160"/>
+      <c r="A13" s="132"/>
+      <c r="B13" s="156"/>
       <c r="C13" s="63" t="s">
         <v>34</v>
       </c>
@@ -10261,8 +10782,8 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="138"/>
-      <c r="B14" s="160"/>
+      <c r="A14" s="132"/>
+      <c r="B14" s="156"/>
       <c r="C14" s="60" t="s">
         <v>7</v>
       </c>
@@ -10283,8 +10804,8 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="138"/>
-      <c r="B15" s="160"/>
+      <c r="A15" s="132"/>
+      <c r="B15" s="156"/>
       <c r="C15" s="60" t="s">
         <v>8</v>
       </c>
@@ -10305,8 +10826,8 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="138"/>
-      <c r="B16" s="160"/>
+      <c r="A16" s="132"/>
+      <c r="B16" s="156"/>
       <c r="C16" s="60" t="s">
         <v>9</v>
       </c>
@@ -10325,10 +10846,10 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="137" t="s">
+      <c r="A17" s="131" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="148"/>
+      <c r="B17" s="125"/>
       <c r="C17" s="59" t="s">
         <v>36</v>
       </c>
@@ -10374,8 +10895,8 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="138"/>
-      <c r="B18" s="149"/>
+      <c r="A18" s="132"/>
+      <c r="B18" s="126"/>
       <c r="C18" s="60" t="s">
         <v>7</v>
       </c>
@@ -10396,8 +10917,8 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="138"/>
-      <c r="B19" s="149"/>
+      <c r="A19" s="132"/>
+      <c r="B19" s="126"/>
       <c r="C19" s="60" t="s">
         <v>8</v>
       </c>
@@ -10418,8 +10939,8 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="138"/>
-      <c r="B20" s="149"/>
+      <c r="A20" s="132"/>
+      <c r="B20" s="126"/>
       <c r="C20" s="61" t="s">
         <v>9</v>
       </c>
@@ -10438,8 +10959,8 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="138"/>
-      <c r="B21" s="157"/>
+      <c r="A21" s="132"/>
+      <c r="B21" s="153"/>
       <c r="C21" s="64" t="s">
         <v>37</v>
       </c>
@@ -10485,8 +11006,8 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="138"/>
-      <c r="B22" s="157"/>
+      <c r="A22" s="132"/>
+      <c r="B22" s="153"/>
       <c r="C22" s="60" t="s">
         <v>7</v>
       </c>
@@ -10505,8 +11026,8 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="138"/>
-      <c r="B23" s="157"/>
+      <c r="A23" s="132"/>
+      <c r="B23" s="153"/>
       <c r="C23" s="60" t="s">
         <v>8</v>
       </c>
@@ -10527,8 +11048,8 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="139"/>
-      <c r="B24" s="158"/>
+      <c r="A24" s="133"/>
+      <c r="B24" s="154"/>
       <c r="C24" s="61" t="s">
         <v>9</v>
       </c>
@@ -10547,10 +11068,10 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="161" t="s">
+      <c r="B25" s="157" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="161"/>
+      <c r="C25" s="157"/>
       <c r="D25" s="47">
         <f t="shared" ref="D25:M28" si="6">SUM(D5,D9,D13,D17,D21)</f>
         <v>0</v>
@@ -10728,13 +11249,13 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="109" t="s">
+      <c r="A30" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="162" t="s">
+      <c r="B30" s="158" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="163"/>
+      <c r="C30" s="159"/>
       <c r="D30" s="32">
         <f xml:space="preserve"> D26</f>
         <v>0</v>
@@ -10773,11 +11294,11 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="110"/>
-      <c r="B31" s="164" t="s">
+      <c r="A31" s="106"/>
+      <c r="B31" s="160" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="132"/>
+      <c r="C31" s="140"/>
       <c r="D31" s="38">
         <f xml:space="preserve"> D27</f>
         <v>0</v>
@@ -10816,11 +11337,11 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="110"/>
-      <c r="B32" s="165" t="s">
+      <c r="A32" s="106"/>
+      <c r="B32" s="161" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="134"/>
+      <c r="C32" s="142"/>
       <c r="D32" s="34">
         <f xml:space="preserve"> D28</f>
         <v>0</v>
@@ -10859,7 +11380,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="111"/>
+      <c r="A33" s="107"/>
       <c r="B33" s="145" t="s">
         <v>25</v>
       </c>
@@ -10916,13 +11437,13 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="140" t="s">
+      <c r="A36" s="134" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="129" t="s">
+      <c r="B36" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="130"/>
+      <c r="C36" s="138"/>
       <c r="D36" s="26">
         <f xml:space="preserve"> SUM(D26:H26)</f>
         <v>6</v>
@@ -10937,11 +11458,11 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="141"/>
-      <c r="B37" s="131" t="s">
+      <c r="A37" s="135"/>
+      <c r="B37" s="139" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="132"/>
+      <c r="C37" s="140"/>
       <c r="D37" s="26">
         <f t="shared" ref="D37:D38" si="7" xml:space="preserve"> SUM(D27:H27)</f>
         <v>8</v>
@@ -10956,11 +11477,11 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="141"/>
-      <c r="B38" s="133" t="s">
+      <c r="A38" s="135"/>
+      <c r="B38" s="141" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="134"/>
+      <c r="C38" s="142"/>
       <c r="D38" s="26">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -10975,7 +11496,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="142"/>
+      <c r="A39" s="136"/>
       <c r="B39" s="143" t="s">
         <v>25</v>
       </c>
@@ -10994,13 +11515,13 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="128" t="s">
+      <c r="A41" s="147" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="129" t="s">
+      <c r="B41" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="130"/>
+      <c r="C41" s="138"/>
       <c r="D41" s="31">
         <f xml:space="preserve"> D36</f>
         <v>6</v>
@@ -11011,11 +11532,11 @@
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="128"/>
-      <c r="B42" s="131" t="s">
+      <c r="A42" s="147"/>
+      <c r="B42" s="139" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="132"/>
+      <c r="C42" s="140"/>
       <c r="D42" s="31">
         <f xml:space="preserve"> D37</f>
         <v>8</v>
@@ -11026,11 +11547,11 @@
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="128"/>
-      <c r="B43" s="133" t="s">
+      <c r="A43" s="147"/>
+      <c r="B43" s="141" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="134"/>
+      <c r="C43" s="142"/>
       <c r="D43" s="31">
         <f xml:space="preserve"> D38</f>
         <v>0</v>
@@ -11041,11 +11562,11 @@
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="128"/>
-      <c r="B44" s="135" t="s">
+      <c r="A44" s="147"/>
+      <c r="B44" s="148" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="136"/>
+      <c r="C44" s="149"/>
       <c r="D44" s="31">
         <f xml:space="preserve"> D39</f>
         <v>14</v>
@@ -11057,16 +11578,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="A5:A16"/>
@@ -11081,8 +11592,32 @@
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
wording fix on product tab
</commit_message>
<xml_diff>
--- a/Management/Effort and Velocity.xlsx
+++ b/Management/Effort and Velocity.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-15" windowWidth="25605" windowHeight="14445" tabRatio="295"/>
@@ -15,7 +15,7 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="56">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>23, 25, 27, 29</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
   </si>
 </sst>
 </file>
@@ -1319,6 +1325,30 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1332,12 +1362,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1391,22 +1415,61 @@
     <xf numFmtId="1" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1428,63 +1491,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1532,18 +1538,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1567,6 +1561,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1648,6 +1654,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2142,12 +2149,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="114692592"/>
-        <c:axId val="114693768"/>
+        <c:axId val="153244416"/>
+        <c:axId val="153245952"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="114692592"/>
+        <c:axId val="153244416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2157,14 +2165,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114693768"/>
+        <c:crossAx val="153245952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="114693768"/>
+        <c:axId val="153245952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2175,13 +2183,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114692592"/>
+        <c:crossAx val="153244416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2444,12 +2453,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116229208"/>
-        <c:axId val="115769584"/>
+        <c:axId val="156916352"/>
+        <c:axId val="156930432"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="116229208"/>
+        <c:axId val="156916352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2459,14 +2469,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115769584"/>
+        <c:crossAx val="156930432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="115769584"/>
+        <c:axId val="156930432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2477,7 +2487,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116229208"/>
+        <c:crossAx val="156916352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2746,12 +2756,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115771152"/>
-        <c:axId val="115774288"/>
+        <c:axId val="156951680"/>
+        <c:axId val="156953216"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="115771152"/>
+        <c:axId val="156951680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2761,14 +2772,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115774288"/>
+        <c:crossAx val="156953216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="115774288"/>
+        <c:axId val="156953216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2779,7 +2790,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115771152"/>
+        <c:crossAx val="156951680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3051,12 +3062,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115772328"/>
-        <c:axId val="115770760"/>
+        <c:axId val="153705856"/>
+        <c:axId val="153711744"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="115772328"/>
+        <c:axId val="153705856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3066,14 +3078,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115770760"/>
+        <c:crossAx val="153711744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="115770760"/>
+        <c:axId val="153711744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3084,7 +3096,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115772328"/>
+        <c:crossAx val="153705856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3317,12 +3329,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115770368"/>
-        <c:axId val="115767624"/>
+        <c:axId val="153737472"/>
+        <c:axId val="153751552"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="115770368"/>
+        <c:axId val="153737472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3332,14 +3345,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115767624"/>
+        <c:crossAx val="153751552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="115767624"/>
+        <c:axId val="153751552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3350,7 +3363,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115770368"/>
+        <c:crossAx val="153737472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3583,12 +3596,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115768800"/>
-        <c:axId val="115771936"/>
+        <c:axId val="153776896"/>
+        <c:axId val="153778432"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="115768800"/>
+        <c:axId val="153776896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3598,14 +3612,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115771936"/>
+        <c:crossAx val="153778432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="115771936"/>
+        <c:axId val="153778432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3616,7 +3630,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115768800"/>
+        <c:crossAx val="153776896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3849,12 +3863,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115773504"/>
-        <c:axId val="115774680"/>
+        <c:axId val="156961792"/>
+        <c:axId val="156971776"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="115773504"/>
+        <c:axId val="156961792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3864,14 +3879,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115774680"/>
+        <c:crossAx val="156971776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="115774680"/>
+        <c:axId val="156971776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3882,7 +3897,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115773504"/>
+        <c:crossAx val="156961792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4115,12 +4130,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115775072"/>
-        <c:axId val="115768016"/>
+        <c:axId val="156993024"/>
+        <c:axId val="156994560"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="115775072"/>
+        <c:axId val="156993024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4130,14 +4146,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115768016"/>
+        <c:crossAx val="156994560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="115768016"/>
+        <c:axId val="156994560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4148,7 +4164,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115775072"/>
+        <c:crossAx val="156993024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4441,12 +4457,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="339479432"/>
-        <c:axId val="339475120"/>
+        <c:axId val="158187904"/>
+        <c:axId val="158189440"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="339479432"/>
+        <c:axId val="158187904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4456,14 +4473,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339475120"/>
+        <c:crossAx val="158189440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="339475120"/>
+        <c:axId val="158189440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4474,7 +4491,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339479432"/>
+        <c:crossAx val="158187904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4770,12 +4787,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="339476296"/>
-        <c:axId val="339480608"/>
+        <c:axId val="158796416"/>
+        <c:axId val="158806400"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="339476296"/>
+        <c:axId val="158796416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4785,14 +4803,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339480608"/>
+        <c:crossAx val="158806400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="339480608"/>
+        <c:axId val="158806400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4803,7 +4821,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339476296"/>
+        <c:crossAx val="158796416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5104,12 +5122,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="339476688"/>
-        <c:axId val="339478256"/>
+        <c:axId val="158848128"/>
+        <c:axId val="158849664"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="339476688"/>
+        <c:axId val="158848128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5119,14 +5138,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339478256"/>
+        <c:crossAx val="158849664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="339478256"/>
+        <c:axId val="158849664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5137,7 +5156,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339476688"/>
+        <c:crossAx val="158848128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5193,6 +5212,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5687,12 +5707,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="114686320"/>
-        <c:axId val="114689064"/>
+        <c:axId val="153259008"/>
+        <c:axId val="153281280"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="114686320"/>
+        <c:axId val="153259008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5702,14 +5723,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114689064"/>
+        <c:crossAx val="153281280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="114689064"/>
+        <c:axId val="153281280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5720,13 +5741,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114686320"/>
+        <c:crossAx val="153259008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6013,12 +6035,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="339473552"/>
-        <c:axId val="339470808"/>
+        <c:axId val="158944640"/>
+        <c:axId val="158946432"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="339473552"/>
+        <c:axId val="158944640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6028,14 +6051,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339470808"/>
+        <c:crossAx val="158946432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="339470808"/>
+        <c:axId val="158946432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6046,7 +6069,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339473552"/>
+        <c:crossAx val="158944640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6102,6 +6125,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6596,12 +6620,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="114687104"/>
-        <c:axId val="114687496"/>
+        <c:axId val="153179648"/>
+        <c:axId val="153181184"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="114687104"/>
+        <c:axId val="153179648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6611,14 +6636,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114687496"/>
+        <c:crossAx val="153181184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="114687496"/>
+        <c:axId val="153181184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6629,13 +6654,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114687104"/>
+        <c:crossAx val="153179648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6685,6 +6711,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7179,12 +7206,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116233520"/>
-        <c:axId val="116233912"/>
+        <c:axId val="153206784"/>
+        <c:axId val="153208320"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="116233520"/>
+        <c:axId val="153206784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7194,14 +7222,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116233912"/>
+        <c:crossAx val="153208320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="116233912"/>
+        <c:axId val="153208320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7212,13 +7240,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116233520"/>
+        <c:crossAx val="153206784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7415,12 +7444,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116234696"/>
-        <c:axId val="116236656"/>
+        <c:axId val="155986176"/>
+        <c:axId val="155987968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116234696"/>
+        <c:axId val="155986176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7430,7 +7460,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116236656"/>
+        <c:crossAx val="155987968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7438,7 +7468,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116236656"/>
+        <c:axId val="155987968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7449,7 +7479,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116234696"/>
+        <c:crossAx val="155986176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7506,6 +7536,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7652,12 +7683,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116229992"/>
-        <c:axId val="116231560"/>
+        <c:axId val="156025600"/>
+        <c:axId val="156027136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116229992"/>
+        <c:axId val="156025600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7667,7 +7699,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116231560"/>
+        <c:crossAx val="156027136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7675,7 +7707,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116231560"/>
+        <c:axId val="156027136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7686,13 +7718,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116229992"/>
+        <c:crossAx val="156025600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7742,6 +7775,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7888,12 +7922,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116230384"/>
-        <c:axId val="116232344"/>
+        <c:axId val="156036096"/>
+        <c:axId val="156775168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116230384"/>
+        <c:axId val="156036096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7903,7 +7938,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116232344"/>
+        <c:crossAx val="156775168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7911,7 +7946,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116232344"/>
+        <c:axId val="156775168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7922,13 +7957,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116230384"/>
+        <c:crossAx val="156036096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7978,6 +8014,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -8124,12 +8161,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116232736"/>
-        <c:axId val="116235088"/>
+        <c:axId val="156804608"/>
+        <c:axId val="156806144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116232736"/>
+        <c:axId val="156804608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8139,7 +8177,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116235088"/>
+        <c:crossAx val="156806144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8147,7 +8185,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116235088"/>
+        <c:axId val="156806144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8158,13 +8196,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116232736"/>
+        <c:crossAx val="156804608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8427,12 +8466,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116229600"/>
-        <c:axId val="116231168"/>
+        <c:axId val="156901760"/>
+        <c:axId val="156903296"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="116229600"/>
+        <c:axId val="156901760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8442,14 +8482,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116231168"/>
+        <c:crossAx val="156903296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="116231168"/>
+        <c:axId val="156903296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8460,7 +8500,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116229600"/>
+        <c:crossAx val="156901760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9180,7 +9220,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -9215,7 +9255,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -9426,8 +9466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AL36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9436,96 +9476,96 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="D2" s="153" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="154"/>
-      <c r="M2" s="154"/>
-      <c r="N2" s="154"/>
-      <c r="O2" s="155"/>
-      <c r="P2" s="153" t="s">
+      <c r="D2" s="148" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="149"/>
+      <c r="I2" s="149"/>
+      <c r="J2" s="149"/>
+      <c r="K2" s="149"/>
+      <c r="L2" s="149"/>
+      <c r="M2" s="149"/>
+      <c r="N2" s="149"/>
+      <c r="O2" s="161"/>
+      <c r="P2" s="148" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="154"/>
-      <c r="R2" s="154"/>
-      <c r="S2" s="154"/>
-      <c r="T2" s="154"/>
-      <c r="U2" s="154"/>
-      <c r="V2" s="154"/>
-      <c r="W2" s="154"/>
-      <c r="X2" s="172"/>
-      <c r="Y2" s="176" t="s">
+      <c r="Q2" s="149"/>
+      <c r="R2" s="149"/>
+      <c r="S2" s="149"/>
+      <c r="T2" s="149"/>
+      <c r="U2" s="149"/>
+      <c r="V2" s="149"/>
+      <c r="W2" s="149"/>
+      <c r="X2" s="150"/>
+      <c r="Y2" s="154" t="s">
         <v>42</v>
       </c>
-      <c r="Z2" s="172"/>
-      <c r="AA2" s="172"/>
-      <c r="AB2" s="172"/>
-      <c r="AC2" s="172"/>
-      <c r="AD2" s="172"/>
-      <c r="AE2" s="172"/>
-      <c r="AF2" s="172"/>
-      <c r="AG2" s="172"/>
-      <c r="AH2" s="172"/>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="172"/>
-      <c r="AK2" s="172"/>
-      <c r="AL2" s="177"/>
+      <c r="Z2" s="150"/>
+      <c r="AA2" s="150"/>
+      <c r="AB2" s="150"/>
+      <c r="AC2" s="150"/>
+      <c r="AD2" s="150"/>
+      <c r="AE2" s="150"/>
+      <c r="AF2" s="150"/>
+      <c r="AG2" s="150"/>
+      <c r="AH2" s="150"/>
+      <c r="AI2" s="150"/>
+      <c r="AJ2" s="150"/>
+      <c r="AK2" s="150"/>
+      <c r="AL2" s="155"/>
     </row>
     <row r="3" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="D3" s="151" t="s">
+      <c r="D3" s="159" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="152"/>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="152"/>
-      <c r="J3" s="153" t="s">
+      <c r="E3" s="160"/>
+      <c r="F3" s="160"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
+      <c r="J3" s="148" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="154"/>
-      <c r="L3" s="154"/>
-      <c r="M3" s="154"/>
-      <c r="N3" s="154"/>
-      <c r="O3" s="155"/>
-      <c r="P3" s="153" t="s">
+      <c r="K3" s="149"/>
+      <c r="L3" s="149"/>
+      <c r="M3" s="149"/>
+      <c r="N3" s="149"/>
+      <c r="O3" s="161"/>
+      <c r="P3" s="148" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="154"/>
-      <c r="R3" s="154"/>
-      <c r="S3" s="154"/>
-      <c r="T3" s="154"/>
-      <c r="U3" s="153" t="s">
+      <c r="Q3" s="149"/>
+      <c r="R3" s="149"/>
+      <c r="S3" s="149"/>
+      <c r="T3" s="149"/>
+      <c r="U3" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="154"/>
-      <c r="W3" s="154"/>
-      <c r="X3" s="172"/>
-      <c r="Y3" s="173" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z3" s="174"/>
-      <c r="AA3" s="174"/>
-      <c r="AB3" s="174"/>
-      <c r="AC3" s="174"/>
-      <c r="AD3" s="174"/>
-      <c r="AE3" s="175"/>
-      <c r="AF3" s="173" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG3" s="174"/>
-      <c r="AH3" s="174"/>
-      <c r="AI3" s="174"/>
-      <c r="AJ3" s="174"/>
-      <c r="AK3" s="174"/>
-      <c r="AL3" s="175"/>
+      <c r="V3" s="149"/>
+      <c r="W3" s="149"/>
+      <c r="X3" s="150"/>
+      <c r="Y3" s="151" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z3" s="152"/>
+      <c r="AA3" s="152"/>
+      <c r="AB3" s="152"/>
+      <c r="AC3" s="152"/>
+      <c r="AD3" s="152"/>
+      <c r="AE3" s="153"/>
+      <c r="AF3" s="151" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG3" s="152"/>
+      <c r="AH3" s="152"/>
+      <c r="AI3" s="152"/>
+      <c r="AJ3" s="152"/>
+      <c r="AK3" s="152"/>
+      <c r="AL3" s="153"/>
     </row>
     <row r="4" spans="2:38" x14ac:dyDescent="0.25">
       <c r="D4" s="1">
@@ -9742,7 +9782,7 @@
       </c>
     </row>
     <row r="6" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B6" s="156" t="s">
+      <c r="B6" s="162" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
@@ -9878,7 +9918,7 @@
       </c>
     </row>
     <row r="7" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B7" s="157"/>
+      <c r="B7" s="163"/>
       <c r="C7" s="29" t="s">
         <v>8</v>
       </c>
@@ -10012,7 +10052,7 @@
       </c>
     </row>
     <row r="8" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B8" s="157"/>
+      <c r="B8" s="163"/>
       <c r="C8" s="30" t="s">
         <v>9</v>
       </c>
@@ -10146,7 +10186,7 @@
       </c>
     </row>
     <row r="9" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B9" s="158"/>
+      <c r="B9" s="164"/>
       <c r="C9" s="69" t="s">
         <v>4</v>
       </c>
@@ -10313,7 +10353,7 @@
       <c r="AI10" s="57"/>
     </row>
     <row r="11" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="156" t="s">
+      <c r="B11" s="162" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="28" t="s">
@@ -10460,7 +10500,7 @@
       </c>
     </row>
     <row r="12" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B12" s="157"/>
+      <c r="B12" s="163"/>
       <c r="C12" s="29" t="s">
         <v>8</v>
       </c>
@@ -10605,7 +10645,7 @@
       </c>
     </row>
     <row r="13" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B13" s="157"/>
+      <c r="B13" s="163"/>
       <c r="C13" s="30" t="s">
         <v>9</v>
       </c>
@@ -10750,7 +10790,7 @@
       </c>
     </row>
     <row r="14" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B14" s="158"/>
+      <c r="B14" s="164"/>
       <c r="C14" s="69" t="s">
         <v>4</v>
       </c>
@@ -10928,7 +10968,7 @@
       <c r="AI15" s="57"/>
     </row>
     <row r="16" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B16" s="148" t="s">
+      <c r="B16" s="156" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="82" t="s">
@@ -11076,7 +11116,7 @@
       </c>
     </row>
     <row r="17" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B17" s="149"/>
+      <c r="B17" s="157"/>
       <c r="C17" s="70" t="s">
         <v>8</v>
       </c>
@@ -11222,7 +11262,7 @@
       </c>
     </row>
     <row r="18" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B18" s="149"/>
+      <c r="B18" s="157"/>
       <c r="C18" s="70" t="s">
         <v>9</v>
       </c>
@@ -11368,7 +11408,7 @@
       </c>
     </row>
     <row r="19" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B19" s="150"/>
+      <c r="B19" s="158"/>
       <c r="C19" s="83" t="s">
         <v>4</v>
       </c>
@@ -11514,28 +11554,28 @@
       </c>
     </row>
     <row r="21" spans="2:38" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="161" t="s">
+      <c r="B21" s="167" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="162"/>
-      <c r="D21" s="163">
+      <c r="C21" s="168"/>
+      <c r="D21" s="169">
         <v>1</v>
       </c>
-      <c r="E21" s="164"/>
-      <c r="F21" s="159">
+      <c r="E21" s="170"/>
+      <c r="F21" s="165">
         <v>2</v>
       </c>
-      <c r="G21" s="160"/>
-      <c r="H21" s="170">
+      <c r="G21" s="166"/>
+      <c r="H21" s="176">
         <v>3</v>
       </c>
-      <c r="I21" s="171"/>
+      <c r="I21" s="177"/>
     </row>
     <row r="22" spans="2:38" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="165" t="s">
+      <c r="B22" s="171" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="166"/>
+      <c r="C22" s="172"/>
       <c r="D22" s="95">
         <v>1</v>
       </c>
@@ -11556,7 +11596,7 @@
       </c>
     </row>
     <row r="23" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B23" s="148" t="s">
+      <c r="B23" s="156" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="82" t="s">
@@ -11588,7 +11628,7 @@
       </c>
     </row>
     <row r="24" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B24" s="149"/>
+      <c r="B24" s="157"/>
       <c r="C24" s="70" t="s">
         <v>8</v>
       </c>
@@ -11609,16 +11649,16 @@
         <v>15</v>
       </c>
       <c r="H24" s="98">
-        <f t="shared" ref="H24:H26" si="28" xml:space="preserve"> SUM(Y7:AE7)</f>
+        <f xml:space="preserve"> SUM(Y7:AE7)</f>
         <v>18</v>
       </c>
       <c r="I24" s="91">
-        <f t="shared" ref="I24:I26" si="29" xml:space="preserve"> SUM(AF7:AL7)</f>
+        <f t="shared" ref="I24:I26" si="28" xml:space="preserve"> SUM(AF7:AL7)</f>
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B25" s="149"/>
+      <c r="B25" s="157"/>
       <c r="C25" s="70" t="s">
         <v>9</v>
       </c>
@@ -11635,20 +11675,20 @@
         <v>0</v>
       </c>
       <c r="G25" s="90">
-        <f t="shared" ref="G25:G26" si="30" xml:space="preserve"> SUM(U8:X8)</f>
+        <f t="shared" ref="G25:G26" si="29" xml:space="preserve"> SUM(U8:X8)</f>
         <v>0</v>
       </c>
       <c r="H25" s="98">
+        <f t="shared" ref="H24:H26" si="30" xml:space="preserve"> SUM(Y8:AE8)</f>
+        <v>1</v>
+      </c>
+      <c r="I25" s="91">
         <f t="shared" si="28"/>
-        <v>1</v>
-      </c>
-      <c r="I25" s="91">
-        <f t="shared" si="29"/>
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B26" s="150"/>
+      <c r="B26" s="158"/>
       <c r="C26" s="83" t="s">
         <v>4</v>
       </c>
@@ -11665,15 +11705,15 @@
         <v>14</v>
       </c>
       <c r="G26" s="137">
+        <f t="shared" si="29"/>
+        <v>18</v>
+      </c>
+      <c r="H26" s="142">
         <f t="shared" si="30"/>
-        <v>18</v>
-      </c>
-      <c r="H26" s="142">
+        <v>22</v>
+      </c>
+      <c r="I26" s="143">
         <f t="shared" si="28"/>
-        <v>22</v>
-      </c>
-      <c r="I26" s="143">
-        <f t="shared" si="29"/>
         <v>18</v>
       </c>
     </row>
@@ -11684,7 +11724,7 @@
       <c r="I27" s="57"/>
     </row>
     <row r="28" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B28" s="167" t="s">
+      <c r="B28" s="173" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="82" t="s">
@@ -11716,7 +11756,7 @@
       </c>
     </row>
     <row r="29" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B29" s="168"/>
+      <c r="B29" s="174"/>
       <c r="C29" s="70" t="s">
         <v>8</v>
       </c>
@@ -11746,7 +11786,7 @@
       </c>
     </row>
     <row r="30" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B30" s="168"/>
+      <c r="B30" s="174"/>
       <c r="C30" s="70" t="s">
         <v>9</v>
       </c>
@@ -11776,7 +11816,7 @@
       </c>
     </row>
     <row r="31" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B31" s="169"/>
+      <c r="B31" s="175"/>
       <c r="C31" s="83" t="s">
         <v>4</v>
       </c>
@@ -11812,7 +11852,7 @@
       <c r="I32" s="57"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="148" t="s">
+      <c r="B33" s="156" t="s">
         <v>29</v>
       </c>
       <c r="C33" s="82" t="s">
@@ -11844,7 +11884,7 @@
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="149"/>
+      <c r="B34" s="157"/>
       <c r="C34" s="70" t="s">
         <v>8</v>
       </c>
@@ -11874,7 +11914,7 @@
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="149"/>
+      <c r="B35" s="157"/>
       <c r="C35" s="70" t="s">
         <v>9</v>
       </c>
@@ -11904,7 +11944,7 @@
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="150"/>
+      <c r="B36" s="158"/>
       <c r="C36" s="83" t="s">
         <v>4</v>
       </c>
@@ -11935,12 +11975,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="U3:X3"/>
-    <mergeCell ref="P2:X2"/>
-    <mergeCell ref="Y3:AE3"/>
-    <mergeCell ref="AF3:AL3"/>
-    <mergeCell ref="Y2:AL2"/>
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="J3:O3"/>
@@ -11955,6 +11989,12 @@
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="H21:I21"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="U3:X3"/>
+    <mergeCell ref="P2:X2"/>
+    <mergeCell ref="Y3:AE3"/>
+    <mergeCell ref="AF3:AL3"/>
+    <mergeCell ref="Y2:AL2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -11985,22 +12025,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D1" s="153" t="s">
+      <c r="D1" s="148" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="154"/>
-      <c r="F1" s="154"/>
-      <c r="G1" s="154"/>
-      <c r="H1" s="154"/>
-      <c r="I1" s="155"/>
-      <c r="J1" s="152" t="s">
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="160" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="152"/>
-      <c r="L1" s="152"/>
-      <c r="M1" s="152"/>
-      <c r="N1" s="152"/>
-      <c r="O1" s="178"/>
+      <c r="K1" s="160"/>
+      <c r="L1" s="160"/>
+      <c r="M1" s="160"/>
+      <c r="N1" s="160"/>
+      <c r="O1" s="197"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C2" s="6" t="s">
@@ -12108,10 +12148,10 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="185" t="s">
+      <c r="A5" s="187" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="179">
+      <c r="B5" s="198">
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -12171,8 +12211,8 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="186"/>
-      <c r="B6" s="180"/>
+      <c r="A6" s="188"/>
+      <c r="B6" s="199"/>
       <c r="C6" s="13" t="s">
         <v>7</v>
       </c>
@@ -12196,8 +12236,8 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="186"/>
-      <c r="B7" s="180"/>
+      <c r="A7" s="188"/>
+      <c r="B7" s="199"/>
       <c r="C7" s="13" t="s">
         <v>8</v>
       </c>
@@ -12221,8 +12261,8 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="186"/>
-      <c r="B8" s="180"/>
+      <c r="A8" s="188"/>
+      <c r="B8" s="199"/>
       <c r="C8" s="17" t="s">
         <v>9</v>
       </c>
@@ -12246,8 +12286,8 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="186"/>
-      <c r="B9" s="180"/>
+      <c r="A9" s="188"/>
+      <c r="B9" s="199"/>
       <c r="C9" s="21" t="s">
         <v>16</v>
       </c>
@@ -12305,8 +12345,8 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="186"/>
-      <c r="B10" s="180"/>
+      <c r="A10" s="188"/>
+      <c r="B10" s="199"/>
       <c r="C10" s="13" t="s">
         <v>7</v>
       </c>
@@ -12328,8 +12368,8 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="186"/>
-      <c r="B11" s="180"/>
+      <c r="A11" s="188"/>
+      <c r="B11" s="199"/>
       <c r="C11" s="13" t="s">
         <v>8</v>
       </c>
@@ -12351,8 +12391,8 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="186"/>
-      <c r="B12" s="180"/>
+      <c r="A12" s="188"/>
+      <c r="B12" s="199"/>
       <c r="C12" s="17" t="s">
         <v>9</v>
       </c>
@@ -12374,8 +12414,8 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="186"/>
-      <c r="B13" s="180"/>
+      <c r="A13" s="188"/>
+      <c r="B13" s="199"/>
       <c r="C13" s="21" t="s">
         <v>17</v>
       </c>
@@ -12433,8 +12473,8 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="186"/>
-      <c r="B14" s="180"/>
+      <c r="A14" s="188"/>
+      <c r="B14" s="199"/>
       <c r="C14" s="13" t="s">
         <v>7</v>
       </c>
@@ -12456,8 +12496,8 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="186"/>
-      <c r="B15" s="180"/>
+      <c r="A15" s="188"/>
+      <c r="B15" s="199"/>
       <c r="C15" s="13" t="s">
         <v>8</v>
       </c>
@@ -12479,8 +12519,8 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="186"/>
-      <c r="B16" s="181"/>
+      <c r="A16" s="188"/>
+      <c r="B16" s="200"/>
       <c r="C16" s="17" t="s">
         <v>9</v>
       </c>
@@ -12506,8 +12546,8 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="186"/>
-      <c r="B17" s="179">
+      <c r="A17" s="188"/>
+      <c r="B17" s="198">
         <v>3</v>
       </c>
       <c r="C17" s="21" t="s">
@@ -12567,8 +12607,8 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="186"/>
-      <c r="B18" s="180"/>
+      <c r="A18" s="188"/>
+      <c r="B18" s="199"/>
       <c r="C18" s="13" t="s">
         <v>7</v>
       </c>
@@ -12594,8 +12634,8 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="186"/>
-      <c r="B19" s="180"/>
+      <c r="A19" s="188"/>
+      <c r="B19" s="199"/>
       <c r="C19" s="13" t="s">
         <v>8</v>
       </c>
@@ -12617,8 +12657,8 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="186"/>
-      <c r="B20" s="181"/>
+      <c r="A20" s="188"/>
+      <c r="B20" s="200"/>
       <c r="C20" s="17" t="s">
         <v>9</v>
       </c>
@@ -12640,8 +12680,8 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="186"/>
-      <c r="B21" s="182"/>
+      <c r="A21" s="188"/>
+      <c r="B21" s="201"/>
       <c r="C21" s="21" t="s">
         <v>19</v>
       </c>
@@ -12699,8 +12739,8 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="186"/>
-      <c r="B22" s="183"/>
+      <c r="A22" s="188"/>
+      <c r="B22" s="202"/>
       <c r="C22" s="13" t="s">
         <v>7</v>
       </c>
@@ -12722,8 +12762,8 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="186"/>
-      <c r="B23" s="183"/>
+      <c r="A23" s="188"/>
+      <c r="B23" s="202"/>
       <c r="C23" s="13" t="s">
         <v>8</v>
       </c>
@@ -12747,8 +12787,8 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="187"/>
-      <c r="B24" s="184"/>
+      <c r="A24" s="189"/>
+      <c r="B24" s="203"/>
       <c r="C24" s="17" t="s">
         <v>9</v>
       </c>
@@ -12998,7 +13038,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="148" t="s">
+      <c r="A30" s="156" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="48" t="s">
@@ -13055,7 +13095,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="149"/>
+      <c r="A31" s="157"/>
       <c r="B31" s="50" t="s">
         <v>8</v>
       </c>
@@ -13110,7 +13150,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="149"/>
+      <c r="A32" s="157"/>
       <c r="B32" s="52" t="s">
         <v>9</v>
       </c>
@@ -13165,11 +13205,11 @@
       </c>
     </row>
     <row r="33" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="150"/>
-      <c r="B33" s="199" t="s">
+      <c r="A33" s="158"/>
+      <c r="B33" s="195" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="200"/>
+      <c r="C33" s="196"/>
       <c r="D33" s="35">
         <f xml:space="preserve"> D25</f>
         <v>0.75</v>
@@ -13234,13 +13274,13 @@
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="188" t="s">
+      <c r="A36" s="190" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="191" t="s">
+      <c r="B36" s="179" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="192"/>
+      <c r="C36" s="180"/>
       <c r="D36" s="26">
         <f xml:space="preserve"> SUM(D26:I26)</f>
         <v>2.75</v>
@@ -13255,11 +13295,11 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="189"/>
-      <c r="B37" s="193" t="s">
+      <c r="A37" s="191"/>
+      <c r="B37" s="181" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="194"/>
+      <c r="C37" s="182"/>
       <c r="D37" s="26">
         <f xml:space="preserve"> SUM(D27:I27)</f>
         <v>0</v>
@@ -13274,11 +13314,11 @@
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="189"/>
-      <c r="B38" s="195" t="s">
+      <c r="A38" s="191"/>
+      <c r="B38" s="183" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="196"/>
+      <c r="C38" s="184"/>
       <c r="D38" s="26">
         <f xml:space="preserve"> SUM(D28:I28)</f>
         <v>0</v>
@@ -13293,11 +13333,11 @@
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="190"/>
-      <c r="B39" s="197" t="s">
+      <c r="A39" s="192"/>
+      <c r="B39" s="193" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="198"/>
+      <c r="C39" s="194"/>
       <c r="D39" s="26">
         <f xml:space="preserve"> SUM(D25:I25)</f>
         <v>2.75</v>
@@ -13312,13 +13352,13 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="201" t="s">
+      <c r="A41" s="178" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="191" t="s">
+      <c r="B41" s="179" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="192"/>
+      <c r="C41" s="180"/>
       <c r="D41" s="31">
         <f xml:space="preserve"> D36</f>
         <v>2.75</v>
@@ -13329,11 +13369,11 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="201"/>
-      <c r="B42" s="193" t="s">
+      <c r="A42" s="178"/>
+      <c r="B42" s="181" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="194"/>
+      <c r="C42" s="182"/>
       <c r="D42" s="31">
         <f xml:space="preserve"> D37</f>
         <v>0</v>
@@ -13344,11 +13384,11 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="201"/>
-      <c r="B43" s="195" t="s">
+      <c r="A43" s="178"/>
+      <c r="B43" s="183" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="196"/>
+      <c r="C43" s="184"/>
       <c r="D43" s="31">
         <f xml:space="preserve"> D38</f>
         <v>0</v>
@@ -13359,11 +13399,11 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="201"/>
-      <c r="B44" s="202" t="s">
+      <c r="A44" s="178"/>
+      <c r="B44" s="185" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="203"/>
+      <c r="C44" s="186"/>
       <c r="D44" s="31">
         <f xml:space="preserve"> D39</f>
         <v>2.75</v>
@@ -13375,11 +13415,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="B5:B16"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B24"/>
     <mergeCell ref="A5:A24"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="B36:C36"/>
@@ -13388,11 +13428,11 @@
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="A30:A33"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="B5:B16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -13421,19 +13461,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D1" s="153" t="s">
+      <c r="D1" s="148" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="154"/>
-      <c r="F1" s="154"/>
-      <c r="G1" s="154"/>
-      <c r="H1" s="154"/>
-      <c r="I1" s="153" t="s">
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="148" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="154"/>
-      <c r="K1" s="154"/>
-      <c r="L1" s="155"/>
+      <c r="J1" s="149"/>
+      <c r="K1" s="149"/>
+      <c r="L1" s="161"/>
       <c r="M1" s="54"/>
       <c r="N1" s="54"/>
       <c r="O1" s="55"/>
@@ -13535,7 +13575,7 @@
       <c r="P4" s="57"/>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="185" t="s">
+      <c r="A5" s="187" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="204">
@@ -13586,7 +13626,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="186"/>
+      <c r="A6" s="188"/>
       <c r="B6" s="205"/>
       <c r="C6" s="60" t="s">
         <v>7</v>
@@ -13606,7 +13646,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="186"/>
+      <c r="A7" s="188"/>
       <c r="B7" s="205"/>
       <c r="C7" s="60" t="s">
         <v>8</v>
@@ -13632,7 +13672,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="186"/>
+      <c r="A8" s="188"/>
       <c r="B8" s="206"/>
       <c r="C8" s="61" t="s">
         <v>9</v>
@@ -13652,7 +13692,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="186"/>
+      <c r="A9" s="188"/>
       <c r="B9" s="209" t="s">
         <v>32</v>
       </c>
@@ -13701,7 +13741,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="186"/>
+      <c r="A10" s="188"/>
       <c r="B10" s="210"/>
       <c r="C10" s="60" t="s">
         <v>7</v>
@@ -13725,7 +13765,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="186"/>
+      <c r="A11" s="188"/>
       <c r="B11" s="210"/>
       <c r="C11" s="60" t="s">
         <v>8</v>
@@ -13745,7 +13785,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="186"/>
+      <c r="A12" s="188"/>
       <c r="B12" s="210"/>
       <c r="C12" s="61" t="s">
         <v>9</v>
@@ -13765,7 +13805,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="186"/>
+      <c r="A13" s="188"/>
       <c r="B13" s="210"/>
       <c r="C13" s="63" t="s">
         <v>34</v>
@@ -13812,7 +13852,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="186"/>
+      <c r="A14" s="188"/>
       <c r="B14" s="210"/>
       <c r="C14" s="60" t="s">
         <v>7</v>
@@ -13834,7 +13874,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="186"/>
+      <c r="A15" s="188"/>
       <c r="B15" s="210"/>
       <c r="C15" s="60" t="s">
         <v>8</v>
@@ -13856,7 +13896,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="186"/>
+      <c r="A16" s="188"/>
       <c r="B16" s="210"/>
       <c r="C16" s="60" t="s">
         <v>9</v>
@@ -13876,10 +13916,10 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="185" t="s">
+      <c r="A17" s="187" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="179"/>
+      <c r="B17" s="198"/>
       <c r="C17" s="59" t="s">
         <v>36</v>
       </c>
@@ -13925,8 +13965,8 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="186"/>
-      <c r="B18" s="180"/>
+      <c r="A18" s="188"/>
+      <c r="B18" s="199"/>
       <c r="C18" s="60" t="s">
         <v>7</v>
       </c>
@@ -13947,8 +13987,8 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="186"/>
-      <c r="B19" s="180"/>
+      <c r="A19" s="188"/>
+      <c r="B19" s="199"/>
       <c r="C19" s="60" t="s">
         <v>8</v>
       </c>
@@ -13969,8 +14009,8 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="186"/>
-      <c r="B20" s="180"/>
+      <c r="A20" s="188"/>
+      <c r="B20" s="199"/>
       <c r="C20" s="61" t="s">
         <v>9</v>
       </c>
@@ -13989,7 +14029,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="186"/>
+      <c r="A21" s="188"/>
       <c r="B21" s="207"/>
       <c r="C21" s="64" t="s">
         <v>37</v>
@@ -14036,7 +14076,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="186"/>
+      <c r="A22" s="188"/>
       <c r="B22" s="207"/>
       <c r="C22" s="60" t="s">
         <v>7</v>
@@ -14056,7 +14096,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="186"/>
+      <c r="A23" s="188"/>
       <c r="B23" s="207"/>
       <c r="C23" s="60" t="s">
         <v>8</v>
@@ -14078,7 +14118,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="187"/>
+      <c r="A24" s="189"/>
       <c r="B24" s="208"/>
       <c r="C24" s="61" t="s">
         <v>9</v>
@@ -14279,7 +14319,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="148" t="s">
+      <c r="A30" s="156" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="212" t="s">
@@ -14324,11 +14364,11 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="149"/>
+      <c r="A31" s="157"/>
       <c r="B31" s="214" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="194"/>
+      <c r="C31" s="182"/>
       <c r="D31" s="38">
         <f xml:space="preserve"> D27</f>
         <v>0</v>
@@ -14367,11 +14407,11 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="149"/>
+      <c r="A32" s="157"/>
       <c r="B32" s="215" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="196"/>
+      <c r="C32" s="184"/>
       <c r="D32" s="34">
         <f xml:space="preserve"> D28</f>
         <v>0</v>
@@ -14410,11 +14450,11 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="150"/>
-      <c r="B33" s="199" t="s">
+      <c r="A33" s="158"/>
+      <c r="B33" s="195" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="200"/>
+      <c r="C33" s="196"/>
       <c r="D33" s="35">
         <f xml:space="preserve"> D25</f>
         <v>0</v>
@@ -14467,13 +14507,13 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="188" t="s">
+      <c r="A36" s="190" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="191" t="s">
+      <c r="B36" s="179" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="192"/>
+      <c r="C36" s="180"/>
       <c r="D36" s="26">
         <f xml:space="preserve"> SUM(D26:H26)</f>
         <v>6</v>
@@ -14488,11 +14528,11 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="189"/>
-      <c r="B37" s="193" t="s">
+      <c r="A37" s="191"/>
+      <c r="B37" s="181" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="194"/>
+      <c r="C37" s="182"/>
       <c r="D37" s="26">
         <f t="shared" ref="D37:D38" si="7" xml:space="preserve"> SUM(D27:H27)</f>
         <v>8</v>
@@ -14507,11 +14547,11 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="189"/>
-      <c r="B38" s="195" t="s">
+      <c r="A38" s="191"/>
+      <c r="B38" s="183" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="196"/>
+      <c r="C38" s="184"/>
       <c r="D38" s="26">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -14526,11 +14566,11 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="190"/>
-      <c r="B39" s="197" t="s">
+      <c r="A39" s="192"/>
+      <c r="B39" s="193" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="198"/>
+      <c r="C39" s="194"/>
       <c r="D39" s="26">
         <f xml:space="preserve"> SUM(D25:H25)</f>
         <v>14</v>
@@ -14545,13 +14585,13 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="201" t="s">
+      <c r="A41" s="178" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="191" t="s">
+      <c r="B41" s="179" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="192"/>
+      <c r="C41" s="180"/>
       <c r="D41" s="31">
         <f xml:space="preserve"> D36</f>
         <v>6</v>
@@ -14562,11 +14602,11 @@
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="201"/>
-      <c r="B42" s="193" t="s">
+      <c r="A42" s="178"/>
+      <c r="B42" s="181" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="194"/>
+      <c r="C42" s="182"/>
       <c r="D42" s="31">
         <f xml:space="preserve"> D37</f>
         <v>8</v>
@@ -14577,11 +14617,11 @@
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="201"/>
-      <c r="B43" s="195" t="s">
+      <c r="A43" s="178"/>
+      <c r="B43" s="183" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="196"/>
+      <c r="C43" s="184"/>
       <c r="D43" s="31">
         <f xml:space="preserve"> D38</f>
         <v>0</v>
@@ -14592,11 +14632,11 @@
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="201"/>
-      <c r="B44" s="202" t="s">
+      <c r="A44" s="178"/>
+      <c r="B44" s="185" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="203"/>
+      <c r="C44" s="186"/>
       <c r="D44" s="31">
         <f xml:space="preserve"> D39</f>
         <v>14</v>
@@ -14608,6 +14648,16 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="A5:A16"/>
@@ -14622,16 +14672,6 @@
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14658,24 +14698,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D1" s="176" t="s">
+      <c r="D1" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="172"/>
-      <c r="F1" s="172"/>
-      <c r="G1" s="172"/>
-      <c r="H1" s="172"/>
-      <c r="I1" s="172"/>
-      <c r="J1" s="172"/>
-      <c r="K1" s="176" t="s">
+      <c r="E1" s="150"/>
+      <c r="F1" s="150"/>
+      <c r="G1" s="150"/>
+      <c r="H1" s="150"/>
+      <c r="I1" s="150"/>
+      <c r="J1" s="150"/>
+      <c r="K1" s="154" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="172"/>
-      <c r="M1" s="172"/>
-      <c r="N1" s="172"/>
-      <c r="O1" s="172"/>
-      <c r="P1" s="172"/>
-      <c r="Q1" s="177"/>
+      <c r="L1" s="150"/>
+      <c r="M1" s="150"/>
+      <c r="N1" s="150"/>
+      <c r="O1" s="150"/>
+      <c r="P1" s="150"/>
+      <c r="Q1" s="155"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C2" s="6" t="s">
@@ -14800,7 +14840,7 @@
       <c r="A5" s="216" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="223">
+      <c r="B5" s="219">
         <v>12</v>
       </c>
       <c r="C5" s="110" t="s">
@@ -14919,7 +14959,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="217"/>
-      <c r="B8" s="224"/>
+      <c r="B8" s="220"/>
       <c r="C8" s="114" t="s">
         <v>9</v>
       </c>
@@ -14946,7 +14986,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="217"/>
-      <c r="B9" s="225">
+      <c r="B9" s="221">
         <v>15</v>
       </c>
       <c r="C9" s="118" t="s">
@@ -15015,7 +15055,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="217"/>
-      <c r="B10" s="226"/>
+      <c r="B10" s="222"/>
       <c r="C10" s="60" t="s">
         <v>7</v>
       </c>
@@ -15040,7 +15080,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="217"/>
-      <c r="B11" s="226"/>
+      <c r="B11" s="222"/>
       <c r="C11" s="60" t="s">
         <v>8</v>
       </c>
@@ -15065,7 +15105,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="217"/>
-      <c r="B12" s="227"/>
+      <c r="B12" s="223"/>
       <c r="C12" s="114" t="s">
         <v>9</v>
       </c>
@@ -15096,7 +15136,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="217"/>
-      <c r="B13" s="225">
+      <c r="B13" s="221">
         <v>21</v>
       </c>
       <c r="C13" s="119" t="s">
@@ -15165,7 +15205,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="217"/>
-      <c r="B14" s="226"/>
+      <c r="B14" s="222"/>
       <c r="C14" s="60" t="s">
         <v>7</v>
       </c>
@@ -15196,7 +15236,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="217"/>
-      <c r="B15" s="226"/>
+      <c r="B15" s="222"/>
       <c r="C15" s="60" t="s">
         <v>8</v>
       </c>
@@ -15221,7 +15261,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="217"/>
-      <c r="B16" s="227"/>
+      <c r="B16" s="223"/>
       <c r="C16" s="114" t="s">
         <v>9</v>
       </c>
@@ -15246,7 +15286,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="217"/>
-      <c r="B17" s="225">
+      <c r="B17" s="221">
         <v>18</v>
       </c>
       <c r="C17" s="119" t="s">
@@ -15315,7 +15355,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="217"/>
-      <c r="B18" s="226"/>
+      <c r="B18" s="222"/>
       <c r="C18" s="60" t="s">
         <v>7</v>
       </c>
@@ -15346,7 +15386,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="217"/>
-      <c r="B19" s="226"/>
+      <c r="B19" s="222"/>
       <c r="C19" s="60" t="s">
         <v>8</v>
       </c>
@@ -15371,7 +15411,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="217"/>
-      <c r="B20" s="227"/>
+      <c r="B20" s="223"/>
       <c r="C20" s="114" t="s">
         <v>9</v>
       </c>
@@ -15396,7 +15436,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="217"/>
-      <c r="B21" s="228" t="s">
+      <c r="B21" s="224" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="119" t="s">
@@ -15465,7 +15505,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="217"/>
-      <c r="B22" s="229"/>
+      <c r="B22" s="225"/>
       <c r="C22" s="60" t="s">
         <v>7</v>
       </c>
@@ -15490,7 +15530,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="217"/>
-      <c r="B23" s="229"/>
+      <c r="B23" s="225"/>
       <c r="C23" s="60" t="s">
         <v>8</v>
       </c>
@@ -15519,7 +15559,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="217"/>
-      <c r="B24" s="230"/>
+      <c r="B24" s="226"/>
       <c r="C24" s="114" t="s">
         <v>9</v>
       </c>
@@ -15544,7 +15584,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="217"/>
-      <c r="B25" s="228" t="s">
+      <c r="B25" s="224" t="s">
         <v>53</v>
       </c>
       <c r="C25" s="119" t="s">
@@ -15613,7 +15653,7 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="217"/>
-      <c r="B26" s="229"/>
+      <c r="B26" s="225"/>
       <c r="C26" s="60" t="s">
         <v>7</v>
       </c>
@@ -15638,7 +15678,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="217"/>
-      <c r="B27" s="229"/>
+      <c r="B27" s="225"/>
       <c r="C27" s="60" t="s">
         <v>8</v>
       </c>
@@ -15665,7 +15705,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="217"/>
-      <c r="B28" s="230"/>
+      <c r="B28" s="226"/>
       <c r="C28" s="114" t="s">
         <v>9</v>
       </c>
@@ -15690,7 +15730,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="217"/>
-      <c r="B29" s="228">
+      <c r="B29" s="224">
         <v>31</v>
       </c>
       <c r="C29" s="119" t="s">
@@ -15759,7 +15799,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="217"/>
-      <c r="B30" s="229"/>
+      <c r="B30" s="225"/>
       <c r="C30" s="60" t="s">
         <v>7</v>
       </c>
@@ -15784,7 +15824,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="217"/>
-      <c r="B31" s="229"/>
+      <c r="B31" s="225"/>
       <c r="C31" s="60" t="s">
         <v>8</v>
       </c>
@@ -15813,7 +15853,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="218"/>
-      <c r="B32" s="230"/>
+      <c r="B32" s="226"/>
       <c r="C32" s="114" t="s">
         <v>9</v>
       </c>
@@ -15840,7 +15880,7 @@
       <c r="A33" s="216" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="219"/>
+      <c r="B33" s="227"/>
       <c r="C33" s="110" t="s">
         <v>51</v>
       </c>
@@ -15907,7 +15947,7 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="217"/>
-      <c r="B34" s="180"/>
+      <c r="B34" s="199"/>
       <c r="C34" s="60" t="s">
         <v>7</v>
       </c>
@@ -15932,7 +15972,7 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="217"/>
-      <c r="B35" s="180"/>
+      <c r="B35" s="199"/>
       <c r="C35" s="60" t="s">
         <v>8</v>
       </c>
@@ -15959,7 +15999,7 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="217"/>
-      <c r="B36" s="180"/>
+      <c r="B36" s="199"/>
       <c r="C36" s="60" t="s">
         <v>9</v>
       </c>
@@ -15984,7 +16024,7 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="217"/>
-      <c r="B37" s="220"/>
+      <c r="B37" s="228"/>
       <c r="C37" s="110" t="s">
         <v>52</v>
       </c>
@@ -16051,7 +16091,7 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="217"/>
-      <c r="B38" s="221"/>
+      <c r="B38" s="229"/>
       <c r="C38" s="60" t="s">
         <v>7</v>
       </c>
@@ -16076,7 +16116,7 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="217"/>
-      <c r="B39" s="221"/>
+      <c r="B39" s="229"/>
       <c r="C39" s="60" t="s">
         <v>8</v>
       </c>
@@ -16105,7 +16145,7 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="218"/>
-      <c r="B40" s="222"/>
+      <c r="B40" s="230"/>
       <c r="C40" s="114" t="s">
         <v>9</v>
       </c>
@@ -16390,7 +16430,7 @@
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="148" t="s">
+      <c r="A46" s="156" t="s">
         <v>5</v>
       </c>
       <c r="B46" s="212" t="s">
@@ -16456,11 +16496,11 @@
       <c r="R46" s="38"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="149"/>
+      <c r="A47" s="157"/>
       <c r="B47" s="214" t="s">
         <v>8</v>
       </c>
-      <c r="C47" s="194"/>
+      <c r="C47" s="182"/>
       <c r="D47" s="38">
         <f>D43</f>
         <v>0</v>
@@ -16520,11 +16560,11 @@
       <c r="R47" s="38"/>
     </row>
     <row r="48" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="149"/>
+      <c r="A48" s="157"/>
       <c r="B48" s="215" t="s">
         <v>9</v>
       </c>
-      <c r="C48" s="196"/>
+      <c r="C48" s="184"/>
       <c r="D48" s="34">
         <f>D44</f>
         <v>0</v>
@@ -16584,11 +16624,11 @@
       <c r="R48" s="38"/>
     </row>
     <row r="49" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="150"/>
-      <c r="B49" s="199" t="s">
+      <c r="A49" s="158"/>
+      <c r="B49" s="195" t="s">
         <v>25</v>
       </c>
-      <c r="C49" s="200"/>
+      <c r="C49" s="196"/>
       <c r="D49" s="35">
         <f>D41</f>
         <v>0</v>
@@ -16662,13 +16702,13 @@
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="188" t="s">
+      <c r="A52" s="190" t="s">
         <v>24</v>
       </c>
-      <c r="B52" s="191" t="s">
+      <c r="B52" s="179" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="192"/>
+      <c r="C52" s="180"/>
       <c r="D52" s="26">
         <f xml:space="preserve"> SUM(D42:J42)</f>
         <v>3</v>
@@ -16683,11 +16723,11 @@
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="189"/>
-      <c r="B53" s="193" t="s">
+      <c r="A53" s="191"/>
+      <c r="B53" s="181" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="194"/>
+      <c r="C53" s="182"/>
       <c r="D53" s="26">
         <f t="shared" ref="D53:D54" si="14" xml:space="preserve"> SUM(D43:J43)</f>
         <v>18</v>
@@ -16702,11 +16742,11 @@
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="189"/>
-      <c r="B54" s="195" t="s">
+      <c r="A54" s="191"/>
+      <c r="B54" s="183" t="s">
         <v>9</v>
       </c>
-      <c r="C54" s="196"/>
+      <c r="C54" s="184"/>
       <c r="D54" s="26">
         <f t="shared" si="14"/>
         <v>1</v>
@@ -16721,11 +16761,11 @@
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" s="190"/>
-      <c r="B55" s="197" t="s">
+      <c r="A55" s="192"/>
+      <c r="B55" s="193" t="s">
         <v>25</v>
       </c>
-      <c r="C55" s="198"/>
+      <c r="C55" s="194"/>
       <c r="D55" s="26">
         <f xml:space="preserve"> SUM(D41:J41)</f>
         <v>22</v>
@@ -16740,13 +16780,13 @@
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="201" t="s">
+      <c r="A57" s="178" t="s">
         <v>26</v>
       </c>
-      <c r="B57" s="191" t="s">
+      <c r="B57" s="179" t="s">
         <v>7</v>
       </c>
-      <c r="C57" s="192"/>
+      <c r="C57" s="180"/>
       <c r="D57" s="31">
         <f xml:space="preserve"> D52</f>
         <v>3</v>
@@ -16757,11 +16797,11 @@
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" s="201"/>
-      <c r="B58" s="193" t="s">
+      <c r="A58" s="178"/>
+      <c r="B58" s="181" t="s">
         <v>8</v>
       </c>
-      <c r="C58" s="194"/>
+      <c r="C58" s="182"/>
       <c r="D58" s="31">
         <f xml:space="preserve"> D53</f>
         <v>18</v>
@@ -16772,11 +16812,11 @@
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" s="201"/>
-      <c r="B59" s="195" t="s">
+      <c r="A59" s="178"/>
+      <c r="B59" s="183" t="s">
         <v>9</v>
       </c>
-      <c r="C59" s="196"/>
+      <c r="C59" s="184"/>
       <c r="D59" s="31">
         <f xml:space="preserve"> D54</f>
         <v>1</v>
@@ -16787,11 +16827,11 @@
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A60" s="201"/>
-      <c r="B60" s="202" t="s">
+      <c r="A60" s="178"/>
+      <c r="B60" s="185" t="s">
         <v>25</v>
       </c>
-      <c r="C60" s="203"/>
+      <c r="C60" s="186"/>
       <c r="D60" s="31">
         <f xml:space="preserve"> D55</f>
         <v>22</v>
@@ -16806,6 +16846,25 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="K1:Q1"/>
     <mergeCell ref="A5:A32"/>
@@ -16816,25 +16875,6 @@
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="B25:B28"/>
     <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A33:A40"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>